<commit_message>
Get full time data for every master postcode from Google Maps API
</commit_message>
<xml_diff>
--- a/output/distance-matrix.xlsx
+++ b/output/distance-matrix.xlsx
@@ -2959,22 +2959,22 @@
       </c>
       <c r="OH2" s="1" t="inlineStr">
         <is>
+          <t>46300</t>
+        </is>
+      </c>
+      <c r="OI2" s="1" t="inlineStr">
+        <is>
           <t>47000</t>
         </is>
       </c>
-      <c r="OI2" s="1" t="inlineStr">
+      <c r="OJ2" s="1" t="inlineStr">
         <is>
           <t>47100</t>
         </is>
       </c>
-      <c r="OJ2" s="1" t="inlineStr">
+      <c r="OK2" s="1" t="inlineStr">
         <is>
           <t>47200</t>
-        </is>
-      </c>
-      <c r="OK2" s="1" t="inlineStr">
-        <is>
-          <t>47810</t>
         </is>
       </c>
       <c r="OL2" s="1" t="inlineStr">
@@ -12043,7 +12043,7 @@
         <v>9.69060539566809</v>
       </c>
       <c r="BO57" t="n">
-        <v>30.98963770956664</v>
+        <v>10.37416370612696</v>
       </c>
       <c r="BP57" t="n">
         <v>19.96049992949565</v>
@@ -12150,7 +12150,7 @@
         <v>23.24777949786191</v>
       </c>
       <c r="BO58" t="n">
-        <v>26.77284014190543</v>
+        <v>25.48969665589189</v>
       </c>
       <c r="BP58" t="n">
         <v>32.18948465749669</v>
@@ -12257,7 +12257,7 @@
         <v>42.08796381013861</v>
       </c>
       <c r="BO59" t="n">
-        <v>32.03970840198555</v>
+        <v>45.30269112997049</v>
       </c>
       <c r="BP59" t="n">
         <v>50.97461299973481</v>
@@ -12364,7 +12364,7 @@
         <v>47.86571745358282</v>
       </c>
       <c r="BO60" t="n">
-        <v>32.11198666670695</v>
+        <v>52.80456892736903</v>
       </c>
       <c r="BP60" t="n">
         <v>59.25213878579763</v>
@@ -12471,7 +12471,7 @@
         <v>31.96562849643178</v>
       </c>
       <c r="BO61" t="n">
-        <v>14.02823447375854</v>
+        <v>40.34294183930831</v>
       </c>
       <c r="BP61" t="n">
         <v>49.11289404520163</v>
@@ -12578,7 +12578,7 @@
         <v>15.52910214077358</v>
       </c>
       <c r="BO62" t="n">
-        <v>13.10708251440183</v>
+        <v>27.54849211024126</v>
       </c>
       <c r="BP62" t="n">
         <v>38.08908293748495</v>
@@ -12685,7 +12685,7 @@
         <v>17.35384031439332</v>
       </c>
       <c r="BO63" t="n">
-        <v>27.10957065688893</v>
+        <v>19.50829978983919</v>
       </c>
       <c r="BP63" t="n">
         <v>27.12074880091311</v>
@@ -12792,7 +12792,7 @@
         <v>39.4261584481546</v>
       </c>
       <c r="BO64" t="n">
-        <v>47.64642305621314</v>
+        <v>33.79683349379389</v>
       </c>
       <c r="BP64" t="n">
         <v>33.61768529488742</v>
@@ -12899,7 +12899,7 @@
         <v>26.30790925058008</v>
       </c>
       <c r="BO65" t="n">
-        <v>41.33026037859</v>
+        <v>19.47663894086085</v>
       </c>
       <c r="BP65" t="n">
         <v>20.68397710964245</v>
@@ -13006,7 +13006,7 @@
         <v>16.35467704549045</v>
       </c>
       <c r="BO66" t="n">
-        <v>34.54165196330923</v>
+        <v>12.26790663384657</v>
       </c>
       <c r="BP66" t="n">
         <v>18.55614770242378</v>
@@ -13113,7 +13113,7 @@
         <v>0</v>
       </c>
       <c r="BO67" t="n">
-        <v>28.52669462960825</v>
+        <v>13.84509304236583</v>
       </c>
       <c r="BP67" t="n">
         <v>24.76827077747171</v>
@@ -13187,103 +13187,103 @@
         </is>
       </c>
       <c r="BD68" t="n">
-        <v>30.98963770956664</v>
+        <v>10.37416370612696</v>
       </c>
       <c r="BE68" t="n">
-        <v>26.77284014190543</v>
+        <v>25.48969665589189</v>
       </c>
       <c r="BF68" t="n">
-        <v>32.03970840198555</v>
+        <v>45.30269112997049</v>
       </c>
       <c r="BG68" t="n">
-        <v>32.11198666670695</v>
+        <v>52.80456892736903</v>
       </c>
       <c r="BH68" t="n">
-        <v>14.02823447375854</v>
+        <v>40.34294183930831</v>
       </c>
       <c r="BI68" t="n">
-        <v>13.10708251440183</v>
+        <v>27.54849211024126</v>
       </c>
       <c r="BJ68" t="n">
-        <v>27.10957065688893</v>
+        <v>19.50829978983919</v>
       </c>
       <c r="BK68" t="n">
-        <v>47.64642305621314</v>
+        <v>33.79683349379389</v>
       </c>
       <c r="BL68" t="n">
-        <v>41.33026037859</v>
+        <v>19.47663894086085</v>
       </c>
       <c r="BM68" t="n">
-        <v>34.54165196330923</v>
+        <v>12.26790663384657</v>
       </c>
       <c r="BN68" t="n">
-        <v>28.52669462960825</v>
+        <v>13.84509304236583</v>
       </c>
       <c r="BO68" t="n">
         <v>0</v>
       </c>
       <c r="BP68" t="n">
-        <v>50.89710994254619</v>
+        <v>10.93374291138725</v>
       </c>
       <c r="BQ68" t="n">
-        <v>46.71931267352677</v>
+        <v>7.160589464747133</v>
       </c>
       <c r="BR68" t="n">
-        <v>64.03143083485379</v>
+        <v>27.4389938761291</v>
       </c>
       <c r="BS68" t="n">
-        <v>36.96552945758002</v>
+        <v>66.85136190192203</v>
       </c>
       <c r="BT68" t="n">
-        <v>84.51862058830713</v>
+        <v>45.53210515547046</v>
       </c>
       <c r="BU68" t="n">
-        <v>76.89899647209752</v>
+        <v>36.99723325686944</v>
       </c>
       <c r="BV68" t="n">
-        <v>84.24128271311619</v>
+        <v>45.39364579190633</v>
       </c>
       <c r="BW68" t="n">
-        <v>66.15425264174347</v>
+        <v>26.12237412444763</v>
       </c>
       <c r="BX68" t="n">
-        <v>73.11237750754849</v>
+        <v>35.45066624691916</v>
       </c>
       <c r="BY68" t="n">
-        <v>79.56806492507926</v>
+        <v>44.24327465902445</v>
       </c>
       <c r="BZ68" t="n">
-        <v>76.22265659565613</v>
+        <v>36.02562994816445</v>
       </c>
       <c r="CA68" t="n">
-        <v>115.6770774507626</v>
+        <v>76.98367905741534</v>
       </c>
       <c r="CB68" t="n">
-        <v>109.482223701876</v>
+        <v>70.56119791170141</v>
       </c>
       <c r="CC68" t="n">
-        <v>104.2389797827818</v>
+        <v>63.83460779664969</v>
       </c>
       <c r="CD68" t="n">
-        <v>107.2623539379559</v>
+        <v>67.46109464329041</v>
       </c>
       <c r="CE68" t="n">
-        <v>96.25838199109853</v>
+        <v>55.78452452482613</v>
       </c>
       <c r="CF68" t="n">
-        <v>100.8128942076295</v>
+        <v>61.43196765581958</v>
       </c>
       <c r="CG68" t="n">
-        <v>115.2091251027253</v>
+        <v>75.15172753286856</v>
       </c>
       <c r="CH68" t="n">
-        <v>109.1166194468215</v>
+        <v>70.40735996905352</v>
       </c>
       <c r="CI68" t="n">
-        <v>134.1670037029749</v>
+        <v>95.28826598216062</v>
       </c>
       <c r="CJ68" t="n">
-        <v>138.6427290122284</v>
+        <v>101.5598528350852</v>
       </c>
     </row>
     <row r="69">
@@ -13327,7 +13327,7 @@
         <v>24.76827077747171</v>
       </c>
       <c r="BO69" t="n">
-        <v>50.89710994254619</v>
+        <v>10.93374291138725</v>
       </c>
       <c r="BP69" t="n">
         <v>0</v>
@@ -13434,7 +13434,7 @@
         <v>18.704826960172</v>
       </c>
       <c r="BO70" t="n">
-        <v>46.71931267352677</v>
+        <v>7.160589464747133</v>
       </c>
       <c r="BP70" t="n">
         <v>8.876170205152851</v>
@@ -13541,7 +13541,7 @@
         <v>35.65628479328674</v>
       </c>
       <c r="BO71" t="n">
-        <v>64.03143083485379</v>
+        <v>27.4389938761291</v>
       </c>
       <c r="BP71" t="n">
         <v>24.14499260551523</v>
@@ -13648,7 +13648,7 @@
         <v>53.05785114499483</v>
       </c>
       <c r="BO72" t="n">
-        <v>36.96552945758002</v>
+        <v>66.85136190192203</v>
       </c>
       <c r="BP72" t="n">
         <v>77.69864941199286</v>
@@ -13755,7 +13755,7 @@
         <v>55.99192957845099</v>
       </c>
       <c r="BO73" t="n">
-        <v>84.51862058830713</v>
+        <v>45.53210515547046</v>
       </c>
       <c r="BP73" t="n">
         <v>38.26635281238588</v>
@@ -13862,7 +13862,7 @@
         <v>48.51509330404784</v>
       </c>
       <c r="BO74" t="n">
-        <v>76.89899647209752</v>
+        <v>36.99723325686944</v>
       </c>
       <c r="BP74" t="n">
         <v>28.85998472091526</v>
@@ -13969,7 +13969,7 @@
         <v>59.23443183843591</v>
       </c>
       <c r="BO75" t="n">
-        <v>84.24128271311619</v>
+        <v>45.39364579190633</v>
       </c>
       <c r="BP75" t="n">
         <v>34.46652148730223</v>
@@ -14076,7 +14076,7 @@
         <v>37.89246884908309</v>
       </c>
       <c r="BO76" t="n">
-        <v>66.15425264174347</v>
+        <v>26.12237412444763</v>
       </c>
       <c r="BP76" t="n">
         <v>18.38195657941162</v>
@@ -14183,7 +14183,7 @@
         <v>44.65745661860307</v>
       </c>
       <c r="BO77" t="n">
-        <v>73.11237750754849</v>
+        <v>35.45066624691916</v>
       </c>
       <c r="BP77" t="n">
         <v>30.13465271145814</v>
@@ -14290,7 +14290,7 @@
         <v>51.65385477383017</v>
       </c>
       <c r="BO78" t="n">
-        <v>79.56806492507926</v>
+        <v>44.24327465902445</v>
       </c>
       <c r="BP78" t="n">
         <v>40.20406452614202</v>
@@ -14397,7 +14397,7 @@
         <v>49.5920264135323</v>
       </c>
       <c r="BO79" t="n">
-        <v>76.22265659565613</v>
+        <v>36.02562994816445</v>
       </c>
       <c r="BP79" t="n">
         <v>25.33727702730232</v>
@@ -14504,7 +14504,7 @@
         <v>87.18564241212336</v>
       </c>
       <c r="BO80" t="n">
-        <v>115.6770774507626</v>
+        <v>76.98367905741534</v>
       </c>
       <c r="BP80" t="n">
         <v>69.32312496588409</v>
@@ -14611,7 +14611,7 @@
         <v>84.3766612774163</v>
       </c>
       <c r="BO81" t="n">
-        <v>109.482223701876</v>
+        <v>70.56119791170141</v>
       </c>
       <c r="BP81" t="n">
         <v>59.62850652511504</v>
@@ -14718,7 +14718,7 @@
         <v>77.09669214557948</v>
       </c>
       <c r="BO82" t="n">
-        <v>104.2389797827818</v>
+        <v>63.83460779664969</v>
       </c>
       <c r="BP82" t="n">
         <v>53.3495198878222</v>
@@ -14825,7 +14825,7 @@
         <v>81.11038233306905</v>
       </c>
       <c r="BO83" t="n">
-        <v>107.2623539379559</v>
+        <v>67.46109464329041</v>
       </c>
       <c r="BP83" t="n">
         <v>56.63065438805496</v>
@@ -14932,7 +14932,7 @@
         <v>68.23196272435776</v>
       </c>
       <c r="BO84" t="n">
-        <v>96.25838199109853</v>
+        <v>55.78452452482613</v>
       </c>
       <c r="BP84" t="n">
         <v>46.16192526167293</v>
@@ -15039,7 +15039,7 @@
         <v>72.29134281360237</v>
       </c>
       <c r="BO85" t="n">
-        <v>100.8128942076295</v>
+        <v>61.43196765581958</v>
       </c>
       <c r="BP85" t="n">
         <v>53.35458918193726</v>
@@ -15146,7 +15146,7 @@
         <v>86.79588952556033</v>
       </c>
       <c r="BO86" t="n">
-        <v>115.2091251027253</v>
+        <v>75.15172753286856</v>
       </c>
       <c r="BP86" t="n">
         <v>66.14913033161717</v>
@@ -15253,7 +15253,7 @@
         <v>80.61811248639304</v>
       </c>
       <c r="BO87" t="n">
-        <v>109.1166194468215</v>
+        <v>70.40735996905352</v>
       </c>
       <c r="BP87" t="n">
         <v>62.82413852311645</v>
@@ -15360,7 +15360,7 @@
         <v>105.6673223431274</v>
       </c>
       <c r="BO88" t="n">
-        <v>134.1670037029749</v>
+        <v>95.28826598216062</v>
       </c>
       <c r="BP88" t="n">
         <v>87.2980094016024</v>
@@ -15467,7 +15467,7 @@
         <v>110.5185448699061</v>
       </c>
       <c r="BO89" t="n">
-        <v>138.6427290122284</v>
+        <v>101.5598528350852</v>
       </c>
       <c r="BP89" t="n">
         <v>94.78146887266392</v>
@@ -50066,7 +50066,7 @@
         <v>31.21812876811232</v>
       </c>
       <c r="NL363" t="n">
-        <v>23.91245473476584</v>
+        <v>27.33173937147869</v>
       </c>
       <c r="NM363" t="n">
         <v>20.86444789049076</v>
@@ -50132,16 +50132,16 @@
         <v>11.15315652590229</v>
       </c>
       <c r="OH363" t="n">
+        <v>12.31266690130801</v>
+      </c>
+      <c r="OI363" t="n">
         <v>16.21018312729053</v>
       </c>
-      <c r="OI363" t="n">
+      <c r="OJ363" t="n">
         <v>11.35166229401295</v>
       </c>
-      <c r="OJ363" t="n">
+      <c r="OK363" t="n">
         <v>8.437881867951438</v>
-      </c>
-      <c r="OK363" t="n">
-        <v>16.49158977239168</v>
       </c>
       <c r="OL363" t="n">
         <v>28.55101027849537</v>
@@ -50156,7 +50156,7 @@
         <v>20.69223837404132</v>
       </c>
       <c r="OP363" t="n">
-        <v>31.53198498237143</v>
+        <v>31.53198354764007</v>
       </c>
       <c r="OQ363" t="n">
         <v>24.00690330816341</v>
@@ -50224,7 +50224,7 @@
         <v>39.78762219457016</v>
       </c>
       <c r="NL364" t="n">
-        <v>32.52859001920159</v>
+        <v>35.47637755962491</v>
       </c>
       <c r="NM364" t="n">
         <v>28.51294349869761</v>
@@ -50290,16 +50290,16 @@
         <v>19.66898655911044</v>
       </c>
       <c r="OH364" t="n">
+        <v>21.07865187829674</v>
+      </c>
+      <c r="OI364" t="n">
         <v>22.53598413109489</v>
       </c>
-      <c r="OI364" t="n">
+      <c r="OJ364" t="n">
         <v>17.68723551524109</v>
       </c>
-      <c r="OJ364" t="n">
+      <c r="OK364" t="n">
         <v>16.6756429456996</v>
-      </c>
-      <c r="OK364" t="n">
-        <v>24.98017908834223</v>
       </c>
       <c r="OL364" t="n">
         <v>34.01871326105415</v>
@@ -50314,7 +50314,7 @@
         <v>29.44961906364409</v>
       </c>
       <c r="OP364" t="n">
-        <v>39.79160000162474</v>
+        <v>39.7915984616263</v>
       </c>
       <c r="OQ364" t="n">
         <v>29.62025923202396</v>
@@ -50382,7 +50382,7 @@
         <v>46.78583845817123</v>
       </c>
       <c r="NL365" t="n">
-        <v>39.635016974521</v>
+        <v>42.00416359083258</v>
       </c>
       <c r="NM365" t="n">
         <v>34.69837253923389</v>
@@ -50448,16 +50448,16 @@
         <v>26.79352016342717</v>
       </c>
       <c r="OH365" t="n">
+        <v>28.60563480297271</v>
+      </c>
+      <c r="OI365" t="n">
         <v>29.97322818725198</v>
       </c>
-      <c r="OI365" t="n">
+      <c r="OJ365" t="n">
         <v>23.46182754811851</v>
       </c>
-      <c r="OJ365" t="n">
+      <c r="OK365" t="n">
         <v>23.66057349296401</v>
-      </c>
-      <c r="OK365" t="n">
-        <v>31.99629414795935</v>
       </c>
       <c r="OL365" t="n">
         <v>40.98361815363896</v>
@@ -50472,7 +50472,7 @@
         <v>36.99799010654742</v>
       </c>
       <c r="OP365" t="n">
-        <v>47.53257583985823</v>
+        <v>47.53257429788042</v>
       </c>
       <c r="OQ365" t="n">
         <v>34.14414282901403</v>
@@ -50540,7 +50540,7 @@
         <v>47.71489267720162</v>
       </c>
       <c r="NL366" t="n">
-        <v>40.44482346452429</v>
+        <v>44.83899038953432</v>
       </c>
       <c r="NM366" t="n">
         <v>38.87560364943053</v>
@@ -50606,16 +50606,16 @@
         <v>28.58509903200166</v>
       </c>
       <c r="OH366" t="n">
+        <v>28.09304759153115</v>
+      </c>
+      <c r="OI366" t="n">
         <v>22.48269686097515</v>
       </c>
-      <c r="OI366" t="n">
+      <c r="OJ366" t="n">
         <v>29.34264534101995</v>
       </c>
-      <c r="OJ366" t="n">
+      <c r="OK366" t="n">
         <v>26.36791892396908</v>
-      </c>
-      <c r="OK366" t="n">
-        <v>33.70778025680086</v>
       </c>
       <c r="OL366" t="n">
         <v>30.25167078419688</v>
@@ -50630,7 +50630,7 @@
         <v>35.48156528612021</v>
       </c>
       <c r="OP366" t="n">
-        <v>42.1074057529838</v>
+        <v>42.10740390920709</v>
       </c>
       <c r="OQ366" t="n">
         <v>41.90080335157847</v>
@@ -50698,7 +50698,7 @@
         <v>38.82948097728325</v>
       </c>
       <c r="NL367" t="n">
-        <v>31.50579915998402</v>
+        <v>35.00762663690855</v>
       </c>
       <c r="NM367" t="n">
         <v>28.4178704388686</v>
@@ -50764,16 +50764,16 @@
         <v>18.82308225048011</v>
       </c>
       <c r="OH367" t="n">
+        <v>19.57438621029571</v>
+      </c>
+      <c r="OI367" t="n">
         <v>19.52534461388999</v>
       </c>
-      <c r="OI367" t="n">
+      <c r="OJ367" t="n">
         <v>18.18628628797919</v>
       </c>
-      <c r="OJ367" t="n">
+      <c r="OK367" t="n">
         <v>16.0967323701332</v>
-      </c>
-      <c r="OK367" t="n">
-        <v>24.15659938104967</v>
       </c>
       <c r="OL367" t="n">
         <v>30.76872533076097</v>
@@ -50788,7 +50788,7 @@
         <v>27.8062482833764</v>
       </c>
       <c r="OP367" t="n">
-        <v>37.39253186264108</v>
+        <v>37.3925302514103</v>
       </c>
       <c r="OQ367" t="n">
         <v>30.59569464032129</v>
@@ -50856,7 +50856,7 @@
         <v>42.68509044286964</v>
       </c>
       <c r="NL368" t="n">
-        <v>36.3430103922543</v>
+        <v>36.70138019375668</v>
       </c>
       <c r="NM368" t="n">
         <v>29.06290809952023</v>
@@ -50922,16 +50922,16 @@
         <v>24.89551585814482</v>
       </c>
       <c r="OH368" t="n">
+        <v>28.28138939180939</v>
+      </c>
+      <c r="OI368" t="n">
         <v>34.82916309582932</v>
       </c>
-      <c r="OI368" t="n">
+      <c r="OJ368" t="n">
         <v>18.55215385156283</v>
       </c>
-      <c r="OJ368" t="n">
+      <c r="OK368" t="n">
         <v>21.84110241705717</v>
-      </c>
-      <c r="OK368" t="n">
-        <v>29.03379155698689</v>
       </c>
       <c r="OL368" t="n">
         <v>47.090236762241</v>
@@ -50946,7 +50946,7 @@
         <v>36.03158923143667</v>
       </c>
       <c r="OP368" t="n">
-        <v>48.71618362833904</v>
+        <v>48.71618246062985</v>
       </c>
       <c r="OQ368" t="n">
         <v>25.28105917061764</v>
@@ -51014,7 +51014,7 @@
         <v>41.92336918301194</v>
       </c>
       <c r="NL369" t="n">
-        <v>36.12020663575544</v>
+        <v>35.55509758436138</v>
       </c>
       <c r="NM369" t="n">
         <v>28.05440516454593</v>
@@ -51080,16 +51080,16 @@
         <v>25.83792699413928</v>
       </c>
       <c r="OH369" t="n">
+        <v>29.64299702132646</v>
+      </c>
+      <c r="OI369" t="n">
         <v>37.74544411887438</v>
       </c>
-      <c r="OI369" t="n">
+      <c r="OJ369" t="n">
         <v>18.72015841744752</v>
       </c>
-      <c r="OJ369" t="n">
+      <c r="OK369" t="n">
         <v>23.06166008731209</v>
-      </c>
-      <c r="OK369" t="n">
-        <v>29.26630511125472</v>
       </c>
       <c r="OL369" t="n">
         <v>50.15913432688987</v>
@@ -51104,7 +51104,7 @@
         <v>36.79745747199557</v>
       </c>
       <c r="OP369" t="n">
-        <v>49.99644238330549</v>
+        <v>49.99644138086828</v>
       </c>
       <c r="OQ369" t="n">
         <v>22.72650088198625</v>
@@ -51172,7 +51172,7 @@
         <v>46.54228203852004</v>
       </c>
       <c r="NL370" t="n">
-        <v>41.34694708719829</v>
+        <v>39.88617025743289</v>
       </c>
       <c r="NM370" t="n">
         <v>32.72845533590535</v>
@@ -51238,16 +51238,16 @@
         <v>32.11768848002415</v>
       </c>
       <c r="OH370" t="n">
+        <v>36.1032387941657</v>
+      </c>
+      <c r="OI370" t="n">
         <v>44.79546248013963</v>
       </c>
-      <c r="OI370" t="n">
+      <c r="OJ370" t="n">
         <v>24.71780185812595</v>
       </c>
-      <c r="OJ370" t="n">
+      <c r="OK370" t="n">
         <v>29.55060030516367</v>
-      </c>
-      <c r="OK370" t="n">
-        <v>34.99698929754675</v>
       </c>
       <c r="OL370" t="n">
         <v>57.22774966438286</v>
@@ -51262,7 +51262,7 @@
         <v>42.7979390804282</v>
       </c>
       <c r="OP370" t="n">
-        <v>56.23729982546006</v>
+        <v>56.23729893616719</v>
       </c>
       <c r="OQ370" t="n">
         <v>25.79854428711469</v>
@@ -51330,7 +51330,7 @@
         <v>55.73726135955316</v>
       </c>
       <c r="NL371" t="n">
-        <v>52.30768155216666</v>
+        <v>48.90145260398944</v>
       </c>
       <c r="NM371" t="n">
         <v>43.1754694204127</v>
@@ -51396,16 +51396,16 @@
         <v>46.10439144888586</v>
       </c>
       <c r="OH371" t="n">
+        <v>50.34103820440826</v>
+      </c>
+      <c r="OI371" t="n">
         <v>60.74185755383225</v>
       </c>
-      <c r="OI371" t="n">
+      <c r="OJ371" t="n">
         <v>38.6482971102602</v>
       </c>
-      <c r="OJ371" t="n">
+      <c r="OK371" t="n">
         <v>44.17487967756728</v>
-      </c>
-      <c r="OK371" t="n">
-        <v>47.53945438684443</v>
       </c>
       <c r="OL371" t="n">
         <v>73.13946856268083</v>
@@ -51420,7 +51420,7 @@
         <v>55.56172177869696</v>
       </c>
       <c r="OP371" t="n">
-        <v>69.20704454708716</v>
+        <v>69.20704401037412</v>
       </c>
       <c r="OQ371" t="n">
         <v>34.09259689233003</v>
@@ -51488,7 +51488,7 @@
         <v>55.99308630032092</v>
       </c>
       <c r="NL372" t="n">
-        <v>49.02110582050226</v>
+        <v>50.73372355257467</v>
       </c>
       <c r="NM372" t="n">
         <v>43.19561913249778</v>
@@ -51554,16 +51554,16 @@
         <v>36.34400241069962</v>
       </c>
       <c r="OH372" t="n">
+        <v>38.5298104584062</v>
+      </c>
+      <c r="OI372" t="n">
         <v>40.16156165562674</v>
       </c>
-      <c r="OI372" t="n">
+      <c r="OJ372" t="n">
         <v>31.95305628141752</v>
       </c>
-      <c r="OJ372" t="n">
+      <c r="OK372" t="n">
         <v>33.14604671893554</v>
-      </c>
-      <c r="OK372" t="n">
-        <v>41.36892776554819</v>
       </c>
       <c r="OL372" t="n">
         <v>50.86029086312607</v>
@@ -51578,7 +51578,7 @@
         <v>46.90684934385468</v>
       </c>
       <c r="OP372" t="n">
-        <v>57.76399693502781</v>
+        <v>57.76399541271257</v>
       </c>
       <c r="OQ372" t="n">
         <v>40.96917147255102</v>
@@ -51646,7 +51646,7 @@
         <v>61.58866957602505</v>
       </c>
       <c r="NL373" t="n">
-        <v>54.3046116325417</v>
+        <v>57.24946508564211</v>
       </c>
       <c r="NM373" t="n">
         <v>50.12423933009669</v>
@@ -51712,16 +51712,16 @@
         <v>41.47048915714802</v>
       </c>
       <c r="OH373" t="n">
+        <v>42.53393496412129</v>
+      </c>
+      <c r="OI373" t="n">
         <v>40.29305415573404</v>
       </c>
-      <c r="OI373" t="n">
+      <c r="OJ373" t="n">
         <v>38.98908800431567</v>
       </c>
-      <c r="OJ373" t="n">
+      <c r="OK373" t="n">
         <v>38.49877305186358</v>
-      </c>
-      <c r="OK373" t="n">
-        <v>46.79405227604212</v>
       </c>
       <c r="OL373" t="n">
         <v>48.88110065856475</v>
@@ -51736,7 +51736,7 @@
         <v>50.75958047145523</v>
       </c>
       <c r="OP373" t="n">
-        <v>59.51713958859602</v>
+        <v>59.51713784702827</v>
       </c>
       <c r="OQ373" t="n">
         <v>49.80930396784379</v>
@@ -51804,7 +51804,7 @@
         <v>54.97711493908349</v>
       </c>
       <c r="NL374" t="n">
-        <v>48.64793693515476</v>
+        <v>48.91348526676232</v>
       </c>
       <c r="NM374" t="n">
         <v>41.29121523831746</v>
@@ -51870,16 +51870,16 @@
         <v>36.99084799261914</v>
       </c>
       <c r="OH374" t="n">
+        <v>40.13834224963037</v>
+      </c>
+      <c r="OI374" t="n">
         <v>45.04246982006463</v>
       </c>
-      <c r="OI374" t="n">
+      <c r="OJ374" t="n">
         <v>30.85611536596489</v>
       </c>
-      <c r="OJ374" t="n">
+      <c r="OK374" t="n">
         <v>33.86261225204071</v>
-      </c>
-      <c r="OK374" t="n">
-        <v>41.29794527824796</v>
       </c>
       <c r="OL374" t="n">
         <v>56.80823724451088</v>
@@ -51894,7 +51894,7 @@
         <v>48.11048643851047</v>
       </c>
       <c r="OP374" t="n">
-        <v>60.44259043512652</v>
+        <v>60.44258916207625</v>
       </c>
       <c r="OQ374" t="n">
         <v>36.71858450428581</v>
@@ -51962,7 +51962,7 @@
         <v>12.04290605742795</v>
       </c>
       <c r="NL375" t="n">
-        <v>12.90648040470502</v>
+        <v>6.510063105159026</v>
       </c>
       <c r="NM375" t="n">
         <v>9.600997044339652</v>
@@ -52028,16 +52028,16 @@
         <v>20.12148128416784</v>
       </c>
       <c r="OH375" t="n">
+        <v>22.08413533294085</v>
+      </c>
+      <c r="OI375" t="n">
         <v>34.49295067553533</v>
       </c>
-      <c r="OI375" t="n">
+      <c r="OJ375" t="n">
         <v>20.27066953513307</v>
       </c>
-      <c r="OJ375" t="n">
+      <c r="OK375" t="n">
         <v>22.10879446117209</v>
-      </c>
-      <c r="OK375" t="n">
-        <v>15.67548064326493</v>
       </c>
       <c r="OL375" t="n">
         <v>43.27364760786495</v>
@@ -52052,7 +52052,7 @@
         <v>19.64036827303204</v>
       </c>
       <c r="OP375" t="n">
-        <v>30.26586040541633</v>
+        <v>30.26586080376381</v>
       </c>
       <c r="OQ375" t="n">
         <v>11.97160258289897</v>
@@ -52120,7 +52120,7 @@
         <v>0</v>
       </c>
       <c r="NL376" t="n">
-        <v>7.333398446074576</v>
+        <v>6.857397402452671</v>
       </c>
       <c r="NM376" t="n">
         <v>13.88483867046533</v>
@@ -52186,16 +52186,16 @@
         <v>20.12010181243892</v>
       </c>
       <c r="OH376" t="n">
+        <v>19.63516487050132</v>
+      </c>
+      <c r="OI376" t="n">
         <v>29.16732727737413</v>
       </c>
-      <c r="OI376" t="n">
+      <c r="OJ376" t="n">
         <v>24.2985464750796</v>
       </c>
-      <c r="OJ376" t="n">
+      <c r="OK376" t="n">
         <v>23.15619140503483</v>
-      </c>
-      <c r="OK376" t="n">
-        <v>14.81615330492677</v>
       </c>
       <c r="OL376" t="n">
         <v>35.12914138540963</v>
@@ -52210,7 +52210,7 @@
         <v>12.99278057532591</v>
       </c>
       <c r="OP376" t="n">
-        <v>19.37021805527369</v>
+        <v>19.37021884787363</v>
       </c>
       <c r="OQ376" t="n">
         <v>21.7440095845571</v>
@@ -52236,154 +52236,154 @@
         </is>
       </c>
       <c r="MX377" t="n">
-        <v>23.91245473476584</v>
+        <v>27.33173937147869</v>
       </c>
       <c r="MY377" t="n">
-        <v>32.52859001920159</v>
+        <v>35.47637755962491</v>
       </c>
       <c r="MZ377" t="n">
-        <v>39.635016974521</v>
+        <v>42.00416359083258</v>
       </c>
       <c r="NA377" t="n">
-        <v>40.44482346452429</v>
+        <v>44.83899038953432</v>
       </c>
       <c r="NB377" t="n">
-        <v>31.50579915998402</v>
+        <v>35.00762663690855</v>
       </c>
       <c r="NC377" t="n">
-        <v>36.3430103922543</v>
+        <v>36.70138019375668</v>
       </c>
       <c r="ND377" t="n">
-        <v>36.12020663575544</v>
+        <v>35.55509758436138</v>
       </c>
       <c r="NE377" t="n">
-        <v>41.34694708719829</v>
+        <v>39.88617025743289</v>
       </c>
       <c r="NF377" t="n">
-        <v>52.30768155216666</v>
+        <v>48.90145260398944</v>
       </c>
       <c r="NG377" t="n">
-        <v>49.02110582050226</v>
+        <v>50.73372355257467</v>
       </c>
       <c r="NH377" t="n">
-        <v>54.3046116325417</v>
+        <v>57.24946508564211</v>
       </c>
       <c r="NI377" t="n">
-        <v>48.64793693515476</v>
+        <v>48.91348526676232</v>
       </c>
       <c r="NJ377" t="n">
-        <v>12.90648040470502</v>
+        <v>6.510063105159026</v>
       </c>
       <c r="NK377" t="n">
-        <v>7.333398446074576</v>
+        <v>6.857397402452671</v>
       </c>
       <c r="NL377" t="n">
         <v>0</v>
       </c>
       <c r="NM377" t="n">
-        <v>9.132247426389196</v>
+        <v>7.643300711600447</v>
       </c>
       <c r="NN377" t="n">
-        <v>12.24547583280537</v>
+        <v>9.467973809070532</v>
       </c>
       <c r="NO377" t="n">
-        <v>20.55361663871383</v>
+        <v>14.05498639192583</v>
       </c>
       <c r="NP377" t="n">
-        <v>17.44471683024011</v>
+        <v>11.74956352224273</v>
       </c>
       <c r="NQ377" t="n">
-        <v>29.43638543312596</v>
+        <v>22.93900409232871</v>
       </c>
       <c r="NR377" t="n">
-        <v>45.3424569999975</v>
+        <v>39.90676931230361</v>
       </c>
       <c r="NS377" t="n">
-        <v>50.51067373665498</v>
+        <v>45.35743116505918</v>
       </c>
       <c r="NT377" t="n">
-        <v>52.37681684903767</v>
+        <v>58.40343501054578</v>
       </c>
       <c r="NU377" t="n">
-        <v>45.77237030131437</v>
+        <v>51.98776088814652</v>
       </c>
       <c r="NV377" t="n">
-        <v>41.62703294281629</v>
+        <v>47.77402836943735</v>
       </c>
       <c r="NW377" t="n">
-        <v>60.55089449844331</v>
+        <v>66.24747677967791</v>
       </c>
       <c r="NX377" t="n">
-        <v>124.7120086385717</v>
+        <v>130.9977206549329</v>
       </c>
       <c r="NY377" t="n">
-        <v>112.0275750818917</v>
+        <v>118.3201816392672</v>
       </c>
       <c r="NZ377" t="n">
-        <v>105.1669240998344</v>
+        <v>111.3296372178933</v>
       </c>
       <c r="OA377" t="n">
-        <v>83.82673949152223</v>
+        <v>89.81168392138724</v>
       </c>
       <c r="OB377" t="n">
-        <v>72.04263218268814</v>
+        <v>77.91837210688794</v>
       </c>
       <c r="OC377" t="n">
-        <v>47.89550145598868</v>
+        <v>54.17424016721553</v>
       </c>
       <c r="OD377" t="n">
-        <v>52.25020421399815</v>
+        <v>57.96679381247997</v>
       </c>
       <c r="OE377" t="n">
-        <v>51.25362626071195</v>
+        <v>56.63052205200047</v>
       </c>
       <c r="OF377" t="n">
-        <v>9.833846140068511</v>
+        <v>13.93310290135445</v>
       </c>
       <c r="OG377" t="n">
-        <v>12.86982506612676</v>
+        <v>16.30028086156909</v>
       </c>
       <c r="OH377" t="n">
-        <v>22.84332134889569</v>
+        <v>17.23511071089795</v>
       </c>
       <c r="OI377" t="n">
-        <v>17.79182961251228</v>
+        <v>28.90147295331241</v>
       </c>
       <c r="OJ377" t="n">
-        <v>15.97453919839341</v>
+        <v>18.7807116137732</v>
       </c>
       <c r="OK377" t="n">
-        <v>7.656945560449512</v>
+        <v>18.91808199046341</v>
       </c>
       <c r="OL377" t="n">
-        <v>30.51551524989133</v>
+        <v>37.01711659437225</v>
       </c>
       <c r="OM377" t="n">
-        <v>38.22059816726475</v>
+        <v>44.48379375656454</v>
       </c>
       <c r="ON377" t="n">
-        <v>33.13215229355873</v>
+        <v>39.60467335755997</v>
       </c>
       <c r="OO377" t="n">
-        <v>6.944829349184612</v>
+        <v>13.40173829585335</v>
       </c>
       <c r="OP377" t="n">
-        <v>18.02967411192094</v>
+        <v>23.81138292074619</v>
       </c>
       <c r="OQ377" t="n">
-        <v>18.47040353933542</v>
+        <v>14.88661294438268</v>
       </c>
       <c r="OR377" t="n">
-        <v>27.37873787599867</v>
+        <v>23.41444484645461</v>
       </c>
       <c r="OS377" t="n">
-        <v>38.37050164766071</v>
+        <v>33.50643538169317</v>
       </c>
       <c r="OT377" t="n">
-        <v>6.132986242918765</v>
+        <v>10.90709615854646</v>
       </c>
       <c r="OU377" t="n">
-        <v>16.92699002249816</v>
+        <v>23.38478275615603</v>
       </c>
     </row>
     <row r="378">
@@ -52436,7 +52436,7 @@
         <v>13.88483867046533</v>
       </c>
       <c r="NL378" t="n">
-        <v>9.132247426389196</v>
+        <v>7.643300711600447</v>
       </c>
       <c r="NM378" t="n">
         <v>0</v>
@@ -52502,16 +52502,16 @@
         <v>10.63235498432611</v>
       </c>
       <c r="OH378" t="n">
+        <v>13.17348271701523</v>
+      </c>
+      <c r="OI378" t="n">
         <v>26.06804239617902</v>
       </c>
-      <c r="OI378" t="n">
+      <c r="OJ378" t="n">
         <v>11.28392456572946</v>
       </c>
-      <c r="OJ378" t="n">
+      <c r="OK378" t="n">
         <v>12.50847451243204</v>
-      </c>
-      <c r="OK378" t="n">
-        <v>6.957618606044848</v>
       </c>
       <c r="OL378" t="n">
         <v>36.15343498079947</v>
@@ -52526,7 +52526,7 @@
         <v>13.57199049330612</v>
       </c>
       <c r="OP378" t="n">
-        <v>26.64392671010039</v>
+        <v>26.6439264970733</v>
       </c>
       <c r="OQ378" t="n">
         <v>9.504954504205804</v>
@@ -52594,7 +52594,7 @@
         <v>16.18690171331687</v>
       </c>
       <c r="NL379" t="n">
-        <v>12.24547583280537</v>
+        <v>9.467973809070532</v>
       </c>
       <c r="NM379" t="n">
         <v>3.279895947509049</v>
@@ -52660,16 +52660,16 @@
         <v>12.61657670981962</v>
       </c>
       <c r="OH379" t="n">
+        <v>15.73381324557645</v>
+      </c>
+      <c r="OI379" t="n">
         <v>28.71641400908567</v>
       </c>
-      <c r="OI379" t="n">
+      <c r="OJ379" t="n">
         <v>11.21628135258284</v>
       </c>
-      <c r="OJ379" t="n">
+      <c r="OK379" t="n">
         <v>13.85254185978611</v>
-      </c>
-      <c r="OK379" t="n">
-        <v>9.860401371793374</v>
       </c>
       <c r="OL379" t="n">
         <v>39.159778138541</v>
@@ -52684,7 +52684,7 @@
         <v>16.83537214446994</v>
       </c>
       <c r="OP379" t="n">
-        <v>29.91019958808815</v>
+        <v>29.91019939562835</v>
       </c>
       <c r="OQ379" t="n">
         <v>6.252437473731589</v>
@@ -52752,7 +52752,7 @@
         <v>17.59751292293053</v>
       </c>
       <c r="NL380" t="n">
-        <v>20.55361663871383</v>
+        <v>14.05498639192583</v>
       </c>
       <c r="NM380" t="n">
         <v>17.53032776052079</v>
@@ -52818,16 +52818,16 @@
         <v>28.1507533802286</v>
       </c>
       <c r="OH380" t="n">
+        <v>30.24601848621955</v>
+      </c>
+      <c r="OI380" t="n">
         <v>42.62568333374519</v>
       </c>
-      <c r="OI380" t="n">
+      <c r="OJ380" t="n">
         <v>27.42834277576236</v>
       </c>
-      <c r="OJ380" t="n">
+      <c r="OK380" t="n">
         <v>29.9377644219226</v>
-      </c>
-      <c r="OK380" t="n">
-        <v>23.83479221606745</v>
       </c>
       <c r="OL380" t="n">
         <v>51.0689888764135</v>
@@ -52842,7 +52842,7 @@
         <v>27.45466076786366</v>
       </c>
       <c r="OP380" t="n">
-        <v>36.87240344349247</v>
+        <v>36.8724041120022</v>
       </c>
       <c r="OQ380" t="n">
         <v>16.67454669704341</v>
@@ -52910,7 +52910,7 @@
         <v>17.99356437669114</v>
       </c>
       <c r="NL381" t="n">
-        <v>17.44471683024011</v>
+        <v>11.74956352224273</v>
       </c>
       <c r="NM381" t="n">
         <v>10.87330435208539</v>
@@ -52976,16 +52976,16 @@
         <v>21.11031698489269</v>
       </c>
       <c r="OH381" t="n">
+        <v>24.02003736908001</v>
+      </c>
+      <c r="OI381" t="n">
         <v>36.94075662161105</v>
       </c>
-      <c r="OI381" t="n">
+      <c r="OJ381" t="n">
         <v>18.99037560631989</v>
       </c>
-      <c r="OJ381" t="n">
+      <c r="OK381" t="n">
         <v>22.30601128599626</v>
-      </c>
-      <c r="OK381" t="n">
-        <v>17.82047071984808</v>
       </c>
       <c r="OL381" t="n">
         <v>46.81424346519258</v>
@@ -53000,7 +53000,7 @@
         <v>23.56117124836214</v>
       </c>
       <c r="OP381" t="n">
-        <v>35.37687317001358</v>
+        <v>35.37687336944715</v>
       </c>
       <c r="OQ381" t="n">
         <v>7.660303645860314</v>
@@ -53068,7 +53068,7 @@
         <v>26.78265696617143</v>
       </c>
       <c r="NL382" t="n">
-        <v>29.43638543312596</v>
+        <v>22.93900409232871</v>
       </c>
       <c r="NM382" t="n">
         <v>24.96305718654304</v>
@@ -53134,16 +53134,16 @@
         <v>35.44780579575596</v>
       </c>
       <c r="OH382" t="n">
+        <v>38.10144743302796</v>
+      </c>
+      <c r="OI382" t="n">
         <v>50.84126379819114</v>
       </c>
-      <c r="OI382" t="n">
+      <c r="OJ382" t="n">
         <v>33.19188333205473</v>
       </c>
-      <c r="OJ382" t="n">
+      <c r="OK382" t="n">
         <v>36.72072096514074</v>
-      </c>
-      <c r="OK382" t="n">
-        <v>31.74395861357146</v>
       </c>
       <c r="OL382" t="n">
         <v>59.87584017902973</v>
@@ -53158,7 +53158,7 @@
         <v>36.23820569521627</v>
       </c>
       <c r="OP382" t="n">
-        <v>46.05921695660545</v>
+        <v>46.0592176131961</v>
       </c>
       <c r="OQ382" t="n">
         <v>20.865133538666</v>
@@ -53226,7 +53226,7 @@
         <v>45.93983224091229</v>
       </c>
       <c r="NL383" t="n">
-        <v>45.3424569999975</v>
+        <v>39.90676931230361</v>
       </c>
       <c r="NM383" t="n">
         <v>37.22294948693085</v>
@@ -53292,16 +53292,16 @@
         <v>44.73601117678374</v>
       </c>
       <c r="OH383" t="n">
+        <v>48.70513053548726</v>
+      </c>
+      <c r="OI383" t="n">
         <v>61.30172596624892</v>
       </c>
-      <c r="OI383" t="n">
+      <c r="OJ383" t="n">
         <v>38.78309515427254</v>
       </c>
-      <c r="OJ383" t="n">
+      <c r="OK383" t="n">
         <v>44.23593889549402</v>
-      </c>
-      <c r="OK383" t="n">
-        <v>43.64777934861662</v>
       </c>
       <c r="OL383" t="n">
         <v>72.69485027448722</v>
@@ -53316,7 +53316,7 @@
         <v>50.78513457497659</v>
       </c>
       <c r="OP383" t="n">
-        <v>63.37109996089509</v>
+        <v>63.37110003574004</v>
       </c>
       <c r="OQ383" t="n">
         <v>28.14692449714786</v>
@@ -53384,7 +53384,7 @@
         <v>51.58971205819324</v>
       </c>
       <c r="NL384" t="n">
-        <v>50.51067373665498</v>
+        <v>45.35743116505918</v>
       </c>
       <c r="NM384" t="n">
         <v>42.05626821130833</v>
@@ -53450,16 +53450,16 @@
         <v>48.74973427039319</v>
       </c>
       <c r="OH384" t="n">
+        <v>52.85024895790607</v>
+      </c>
+      <c r="OI384" t="n">
         <v>65.12966413426869</v>
       </c>
-      <c r="OI384" t="n">
+      <c r="OJ384" t="n">
         <v>42.30439350309043</v>
       </c>
-      <c r="OJ384" t="n">
+      <c r="OK384" t="n">
         <v>47.91229503048633</v>
-      </c>
-      <c r="OK384" t="n">
-        <v>48.1870961165827</v>
       </c>
       <c r="OL384" t="n">
         <v>76.84860443841094</v>
@@ -53474,7 +53474,7 @@
         <v>55.61128895346185</v>
       </c>
       <c r="OP384" t="n">
-        <v>68.51446648254252</v>
+        <v>68.51446644979339</v>
       </c>
       <c r="OQ384" t="n">
         <v>32.70597171495756</v>
@@ -53542,7 +53542,7 @@
         <v>53.82436527959677</v>
       </c>
       <c r="NL385" t="n">
-        <v>52.37681684903767</v>
+        <v>58.40343501054578</v>
       </c>
       <c r="NM385" t="n">
         <v>60.31525978674777</v>
@@ -53608,16 +53608,16 @@
         <v>54.65747798744768</v>
       </c>
       <c r="OH385" t="n">
+        <v>50.40311737750042</v>
+      </c>
+      <c r="OI385" t="n">
         <v>40.6890833057524</v>
       </c>
-      <c r="OI385" t="n">
+      <c r="OJ385" t="n">
         <v>62.03324767597061</v>
       </c>
-      <c r="OJ385" t="n">
+      <c r="OK385" t="n">
         <v>56.49159858256399</v>
-      </c>
-      <c r="OK385" t="n">
-        <v>54.23499867426946</v>
       </c>
       <c r="OL385" t="n">
         <v>28.45675116944632</v>
@@ -53632,7 +53632,7 @@
         <v>46.74359530366337</v>
       </c>
       <c r="OP385" t="n">
-        <v>34.63154950022449</v>
+        <v>34.63154901959135</v>
       </c>
       <c r="OQ385" t="n">
         <v>69.63877183928561</v>
@@ -53700,7 +53700,7 @@
         <v>47.90263814704114</v>
       </c>
       <c r="NL386" t="n">
-        <v>45.77237030131437</v>
+        <v>51.98776088814652</v>
       </c>
       <c r="NM386" t="n">
         <v>53.34352422049721</v>
@@ -53766,16 +53766,16 @@
         <v>47.17219700084158</v>
       </c>
       <c r="OH386" t="n">
+        <v>42.92194695530374</v>
+      </c>
+      <c r="OI386" t="n">
         <v>32.85135757465112</v>
       </c>
-      <c r="OI386" t="n">
+      <c r="OJ386" t="n">
         <v>54.47492031097266</v>
       </c>
-      <c r="OJ386" t="n">
+      <c r="OK386" t="n">
         <v>48.88623503507016</v>
-      </c>
-      <c r="OK386" t="n">
-        <v>47.05538344664005</v>
       </c>
       <c r="OL386" t="n">
         <v>20.57045423085658</v>
@@ -53790,7 +53790,7 @@
         <v>39.8034649157076</v>
       </c>
       <c r="OP386" t="n">
-        <v>28.53292590380833</v>
+        <v>28.53292512797516</v>
       </c>
       <c r="OQ386" t="n">
         <v>62.54277907499416</v>
@@ -53858,7 +53858,7 @@
         <v>43.54792816498777</v>
       </c>
       <c r="NL387" t="n">
-        <v>41.62703294281629</v>
+        <v>47.77402836943735</v>
       </c>
       <c r="NM387" t="n">
         <v>49.39432152277862</v>
@@ -53924,16 +53924,16 @@
         <v>43.66746710666825</v>
       </c>
       <c r="OH387" t="n">
+        <v>39.41379683807347</v>
+      </c>
+      <c r="OI387" t="n">
         <v>30.10236587932901</v>
       </c>
-      <c r="OI387" t="n">
+      <c r="OJ387" t="n">
         <v>51.06281255339238</v>
       </c>
-      <c r="OJ387" t="n">
+      <c r="OK387" t="n">
         <v>45.54630745009298</v>
-      </c>
-      <c r="OK387" t="n">
-        <v>43.24954028262403</v>
       </c>
       <c r="OL387" t="n">
         <v>18.25730098003725</v>
@@ -53948,7 +53948,7 @@
         <v>35.82559150420402</v>
       </c>
       <c r="OP387" t="n">
-        <v>24.19057487955794</v>
+        <v>24.19057417526572</v>
       </c>
       <c r="OQ387" t="n">
         <v>58.67931615980193</v>
@@ -54016,7 +54016,7 @@
         <v>67.078145303097</v>
       </c>
       <c r="NL388" t="n">
-        <v>60.55089449844331</v>
+        <v>66.24747677967791</v>
       </c>
       <c r="NM388" t="n">
         <v>61.88213278118528</v>
@@ -54082,16 +54082,16 @@
         <v>51.27319371849463</v>
       </c>
       <c r="OH388" t="n">
+        <v>49.14329445481175</v>
+      </c>
+      <c r="OI388" t="n">
         <v>37.9170679558581</v>
       </c>
-      <c r="OI388" t="n">
+      <c r="OJ388" t="n">
         <v>54.25382741118214</v>
       </c>
-      <c r="OJ388" t="n">
+      <c r="OK388" t="n">
         <v>50.01030693742152</v>
-      </c>
-      <c r="OK388" t="n">
-        <v>55.52154840889894</v>
       </c>
       <c r="OL388" t="n">
         <v>36.3375681991263</v>
@@ -54106,7 +54106,7 @@
         <v>54.09381802257371</v>
       </c>
       <c r="OP388" t="n">
-        <v>54.50507807783873</v>
+        <v>54.50507614813898</v>
       </c>
       <c r="OQ388" t="n">
         <v>66.86453438613836</v>
@@ -54174,7 +54174,7 @@
         <v>130.1186875687013</v>
       </c>
       <c r="NL389" t="n">
-        <v>124.7120086385717</v>
+        <v>130.9977206549329</v>
       </c>
       <c r="NM389" t="n">
         <v>127.9907004292011</v>
@@ -54240,16 +54240,16 @@
         <v>117.6940714670469</v>
       </c>
       <c r="OH389" t="n">
+        <v>114.8340814261667</v>
+      </c>
+      <c r="OI389" t="n">
         <v>102.1998048761191</v>
       </c>
-      <c r="OI389" t="n">
+      <c r="OJ389" t="n">
         <v>121.676879104274</v>
       </c>
-      <c r="OJ389" t="n">
+      <c r="OK389" t="n">
         <v>116.9626044099027</v>
-      </c>
-      <c r="OK389" t="n">
-        <v>121.1990960452153</v>
       </c>
       <c r="OL389" t="n">
         <v>95.15800113728211</v>
@@ -54264,7 +54264,7 @@
         <v>117.7996899353037</v>
       </c>
       <c r="OP389" t="n">
-        <v>113.2276508301453</v>
+        <v>113.2276492183155</v>
       </c>
       <c r="OQ389" t="n">
         <v>134.0900428516518</v>
@@ -54332,7 +54332,7 @@
         <v>117.4280313025028</v>
       </c>
       <c r="NL390" t="n">
-        <v>112.0275750818917</v>
+        <v>118.3201816392672</v>
       </c>
       <c r="NM390" t="n">
         <v>115.367499952048</v>
@@ -54398,16 +54398,16 @@
         <v>105.1049398467503</v>
       </c>
       <c r="OH390" t="n">
+        <v>102.2042719417844</v>
+      </c>
+      <c r="OI390" t="n">
         <v>89.53937196418444</v>
       </c>
-      <c r="OI390" t="n">
+      <c r="OJ390" t="n">
         <v>109.1975723454027</v>
       </c>
-      <c r="OJ390" t="n">
+      <c r="OK390" t="n">
         <v>104.4238666042248</v>
-      </c>
-      <c r="OK390" t="n">
-        <v>108.5604948329179</v>
       </c>
       <c r="OL390" t="n">
         <v>82.47802161853738</v>
@@ -54422,7 +54422,7 @@
         <v>105.1130960199391</v>
       </c>
       <c r="OP390" t="n">
-        <v>100.5896680480641</v>
+        <v>100.5896664243062</v>
       </c>
       <c r="OQ390" t="n">
         <v>121.5645015114527</v>
@@ -54490,7 +54490,7 @@
         <v>110.9066436156113</v>
       </c>
       <c r="NL391" t="n">
-        <v>105.1669240998344</v>
+        <v>111.3296372178933</v>
       </c>
       <c r="NM391" t="n">
         <v>107.9199187346679</v>
@@ -54556,16 +54556,16 @@
         <v>97.49403833635567</v>
       </c>
       <c r="OH391" t="n">
+        <v>94.8241405061255</v>
+      </c>
+      <c r="OI391" t="n">
         <v>82.43132347787902</v>
       </c>
-      <c r="OI391" t="n">
+      <c r="OJ391" t="n">
         <v>101.1614410411764</v>
       </c>
-      <c r="OJ391" t="n">
+      <c r="OK391" t="n">
         <v>96.59911568215772</v>
-      </c>
-      <c r="OK391" t="n">
-        <v>101.2251075185475</v>
       </c>
       <c r="OL391" t="n">
         <v>76.39370298724894</v>
@@ -54580,7 +54580,7 @@
         <v>98.31971087945172</v>
       </c>
       <c r="OP391" t="n">
-        <v>94.87967703466988</v>
+        <v>94.87967532092564</v>
       </c>
       <c r="OQ391" t="n">
         <v>113.6668031588408</v>
@@ -54648,7 +54648,7 @@
         <v>89.92932460248143</v>
       </c>
       <c r="NL392" t="n">
-        <v>83.82673949152223</v>
+        <v>89.81168392138724</v>
       </c>
       <c r="NM392" t="n">
         <v>85.96302313721777</v>
@@ -54714,16 +54714,16 @@
         <v>75.43104387318816</v>
       </c>
       <c r="OH392" t="n">
+        <v>72.98937529344718</v>
+      </c>
+      <c r="OI392" t="n">
         <v>60.98371688216066</v>
       </c>
-      <c r="OI392" t="n">
+      <c r="OJ392" t="n">
         <v>78.76477412478872</v>
       </c>
-      <c r="OJ392" t="n">
+      <c r="OK392" t="n">
         <v>74.36290386549057</v>
-      </c>
-      <c r="OK392" t="n">
-        <v>79.4020145729573</v>
       </c>
       <c r="OL392" t="n">
         <v>56.44811038964955</v>
@@ -54738,7 +54738,7 @@
         <v>77.1056379003678</v>
       </c>
       <c r="OP392" t="n">
-        <v>75.17025999515091</v>
+        <v>75.1702581719654</v>
       </c>
       <c r="OQ392" t="n">
         <v>91.3366591158269</v>
@@ -54806,7 +54806,7 @@
         <v>78.32829590256512</v>
       </c>
       <c r="NL393" t="n">
-        <v>72.04263218268814</v>
+        <v>77.91837210688794</v>
       </c>
       <c r="NM393" t="n">
         <v>73.86049162606061</v>
@@ -54872,16 +54872,16 @@
         <v>63.2927250226998</v>
       </c>
       <c r="OH393" t="n">
+        <v>60.96668988259839</v>
+      </c>
+      <c r="OI393" t="n">
         <v>49.22669048065715</v>
       </c>
-      <c r="OI393" t="n">
+      <c r="OJ393" t="n">
         <v>66.49901658305473</v>
       </c>
-      <c r="OJ393" t="n">
+      <c r="OK393" t="n">
         <v>62.15216493368043</v>
-      </c>
-      <c r="OK393" t="n">
-        <v>67.37285204182045</v>
       </c>
       <c r="OL393" t="n">
         <v>45.77761664281584</v>
@@ -54896,7 +54896,7 @@
         <v>65.41510694395888</v>
       </c>
       <c r="OP393" t="n">
-        <v>64.42567892847572</v>
+        <v>64.42567705161842</v>
       </c>
       <c r="OQ393" t="n">
         <v>79.08594042087415</v>
@@ -54964,7 +54964,7 @@
         <v>53.51016784195968</v>
       </c>
       <c r="NL394" t="n">
-        <v>47.89550145598868</v>
+        <v>54.17424016721553</v>
       </c>
       <c r="NM394" t="n">
         <v>51.49097743969767</v>
@@ -55030,16 +55030,16 @@
         <v>41.56856073974672</v>
       </c>
       <c r="OH394" t="n">
+        <v>38.33101307445015</v>
+      </c>
+      <c r="OI394" t="n">
         <v>25.47235133483689</v>
       </c>
-      <c r="OI394" t="n">
+      <c r="OJ394" t="n">
         <v>46.6626263527158</v>
       </c>
-      <c r="OJ394" t="n">
+      <c r="OK394" t="n">
         <v>41.38730691393158</v>
-      </c>
-      <c r="OK394" t="n">
-        <v>44.59697608130264</v>
       </c>
       <c r="OL394" t="n">
         <v>19.53648443762546</v>
@@ -55054,7 +55054,7 @@
         <v>40.99869221570177</v>
       </c>
       <c r="OP394" t="n">
-        <v>38.25673170115465</v>
+        <v>38.25672986206825</v>
       </c>
       <c r="OQ394" t="n">
         <v>58.41975992711831</v>
@@ -55122,7 +55122,7 @@
         <v>58.78170521984111</v>
       </c>
       <c r="NL395" t="n">
-        <v>52.25020421399815</v>
+        <v>57.96679381247997</v>
       </c>
       <c r="NM395" t="n">
         <v>53.71058591382157</v>
@@ -55188,16 +55188,16 @@
         <v>43.12703730521925</v>
       </c>
       <c r="OH395" t="n">
+        <v>40.89556321980829</v>
+      </c>
+      <c r="OI395" t="n">
         <v>29.62651857687093</v>
       </c>
-      <c r="OI395" t="n">
+      <c r="OJ395" t="n">
         <v>46.41352920164212</v>
       </c>
-      <c r="OJ395" t="n">
+      <c r="OK395" t="n">
         <v>41.98360572437431</v>
-      </c>
-      <c r="OK395" t="n">
-        <v>47.28633800481356</v>
       </c>
       <c r="OL395" t="n">
         <v>28.7964042561256</v>
@@ -55212,7 +55212,7 @@
         <v>45.7952196840757</v>
       </c>
       <c r="OP395" t="n">
-        <v>46.58042536441588</v>
+        <v>46.58042342171095</v>
       </c>
       <c r="OQ395" t="n">
         <v>58.96029235507688</v>
@@ -55280,7 +55280,7 @@
         <v>58.08603174989094</v>
       </c>
       <c r="NL396" t="n">
-        <v>51.25362626071195</v>
+        <v>56.63052205200047</v>
       </c>
       <c r="NM396" t="n">
         <v>51.77954603264979</v>
@@ -55346,16 +55346,16 @@
         <v>41.14838227823062</v>
       </c>
       <c r="OH396" t="n">
+        <v>39.4010210041742</v>
+      </c>
+      <c r="OI396" t="n">
         <v>29.30427807982484</v>
       </c>
-      <c r="OI396" t="n">
+      <c r="OJ396" t="n">
         <v>43.63099265649031</v>
       </c>
-      <c r="OJ396" t="n">
+      <c r="OK396" t="n">
         <v>39.64248690013154</v>
-      </c>
-      <c r="OK396" t="n">
-        <v>45.67676240665195</v>
       </c>
       <c r="OL396" t="n">
         <v>30.78767869582044</v>
@@ -55370,7 +55370,7 @@
         <v>45.13103001071075</v>
       </c>
       <c r="OP396" t="n">
-        <v>47.55016400369718</v>
+        <v>47.55016204892787</v>
       </c>
       <c r="OQ396" t="n">
         <v>56.27857811025333</v>
@@ -55438,7 +55438,7 @@
         <v>17.1480168090134</v>
       </c>
       <c r="NL397" t="n">
-        <v>9.833846140068511</v>
+        <v>13.93310290135445</v>
       </c>
       <c r="NM397" t="n">
         <v>9.500433174196234</v>
@@ -55504,16 +55504,16 @@
         <v>3.211226006896681</v>
       </c>
       <c r="OH397" t="n">
+        <v>3.675036839084714</v>
+      </c>
+      <c r="OI397" t="n">
         <v>16.60583853585631</v>
       </c>
-      <c r="OI397" t="n">
+      <c r="OJ397" t="n">
         <v>10.07506377552812</v>
       </c>
-      <c r="OJ397" t="n">
+      <c r="OK397" t="n">
         <v>6.422484399208642</v>
-      </c>
-      <c r="OK397" t="n">
-        <v>2.834429869728361</v>
       </c>
       <c r="OL397" t="n">
         <v>27.25912296867322</v>
@@ -55528,7 +55528,7 @@
         <v>8.10035913815735</v>
       </c>
       <c r="OP397" t="n">
-        <v>21.45953749051091</v>
+        <v>21.45953665135958</v>
       </c>
       <c r="OQ397" t="n">
         <v>17.34003796372285</v>
@@ -55596,7 +55596,7 @@
         <v>20.12010181243892</v>
       </c>
       <c r="NL398" t="n">
-        <v>12.86982506612676</v>
+        <v>16.30028086156909</v>
       </c>
       <c r="NM398" t="n">
         <v>10.63235498432611</v>
@@ -55662,16 +55662,16 @@
         <v>0</v>
       </c>
       <c r="OH398" t="n">
+        <v>4.254473041096979</v>
+      </c>
+      <c r="OI398" t="n">
         <v>16.61671967024451</v>
       </c>
-      <c r="OI398" t="n">
+      <c r="OJ398" t="n">
         <v>7.525252220864362</v>
       </c>
-      <c r="OJ398" t="n">
+      <c r="OK398" t="n">
         <v>3.211258392999594</v>
-      </c>
-      <c r="OK398" t="n">
-        <v>5.339553017252469</v>
       </c>
       <c r="OL398" t="n">
         <v>28.10505186291871</v>
@@ -55686,7 +55686,7 @@
         <v>11.13665910404527</v>
       </c>
       <c r="OP398" t="n">
-        <v>24.16687687868328</v>
+        <v>24.1668759081573</v>
       </c>
       <c r="OQ398" t="n">
         <v>16.94489140394498</v>
@@ -55708,632 +55708,632 @@
       <c r="A399" s="4" t="n"/>
       <c r="B399" s="1" t="inlineStr">
         <is>
-          <t>47000</t>
+          <t>46300</t>
         </is>
       </c>
       <c r="MX399" t="n">
-        <v>16.21018312729053</v>
+        <v>12.31266690130801</v>
       </c>
       <c r="MY399" t="n">
-        <v>22.53598413109489</v>
+        <v>21.07865187829674</v>
       </c>
       <c r="MZ399" t="n">
-        <v>29.97322818725198</v>
+        <v>28.60563480297271</v>
       </c>
       <c r="NA399" t="n">
-        <v>22.48269686097515</v>
+        <v>28.09304759153115</v>
       </c>
       <c r="NB399" t="n">
-        <v>19.52534461388999</v>
+        <v>19.57438621029571</v>
       </c>
       <c r="NC399" t="n">
-        <v>34.82916309582932</v>
+        <v>28.28138939180939</v>
       </c>
       <c r="ND399" t="n">
-        <v>37.74544411887438</v>
+        <v>29.64299702132646</v>
       </c>
       <c r="NE399" t="n">
-        <v>44.79546248013963</v>
+        <v>36.1032387941657</v>
       </c>
       <c r="NF399" t="n">
-        <v>60.74185755383225</v>
+        <v>50.34103820440826</v>
       </c>
       <c r="NG399" t="n">
-        <v>40.16156165562674</v>
+        <v>38.5298104584062</v>
       </c>
       <c r="NH399" t="n">
-        <v>40.29305415573404</v>
+        <v>42.53393496412129</v>
       </c>
       <c r="NI399" t="n">
-        <v>45.04246982006463</v>
+        <v>40.13834224963037</v>
       </c>
       <c r="NJ399" t="n">
-        <v>34.49295067553533</v>
+        <v>22.08413533294085</v>
       </c>
       <c r="NK399" t="n">
-        <v>29.16732727737413</v>
+        <v>19.63516487050132</v>
       </c>
       <c r="NL399" t="n">
-        <v>22.84332134889569</v>
+        <v>17.23511071089795</v>
       </c>
       <c r="NM399" t="n">
-        <v>26.06804239617902</v>
+        <v>13.17348271701523</v>
       </c>
       <c r="NN399" t="n">
-        <v>28.71641400908567</v>
+        <v>15.73381324557645</v>
       </c>
       <c r="NO399" t="n">
-        <v>42.62568333374519</v>
+        <v>30.24601848621955</v>
       </c>
       <c r="NP399" t="n">
-        <v>36.94075662161105</v>
+        <v>24.02003736908001</v>
       </c>
       <c r="NQ399" t="n">
-        <v>50.84126379819114</v>
+        <v>38.10144743302796</v>
       </c>
       <c r="NR399" t="n">
-        <v>61.30172596624892</v>
+        <v>48.70513053548726</v>
       </c>
       <c r="NS399" t="n">
-        <v>65.12966413426869</v>
+        <v>52.85024895790607</v>
       </c>
       <c r="NT399" t="n">
-        <v>40.6890833057524</v>
+        <v>50.40311737750042</v>
       </c>
       <c r="NU399" t="n">
-        <v>32.85135757465112</v>
+        <v>42.92194695530374</v>
       </c>
       <c r="NV399" t="n">
-        <v>30.10236587932901</v>
+        <v>39.41379683807347</v>
       </c>
       <c r="NW399" t="n">
-        <v>37.9170679558581</v>
+        <v>49.14329445481175</v>
       </c>
       <c r="NX399" t="n">
-        <v>102.1998048761191</v>
+        <v>114.8340814261667</v>
       </c>
       <c r="NY399" t="n">
-        <v>89.53937196418444</v>
+        <v>102.2042719417844</v>
       </c>
       <c r="NZ399" t="n">
-        <v>82.43132347787902</v>
+        <v>94.8241405061255</v>
       </c>
       <c r="OA399" t="n">
-        <v>60.98371688216066</v>
+        <v>72.98937529344718</v>
       </c>
       <c r="OB399" t="n">
-        <v>49.22669048065715</v>
+        <v>60.96668988259839</v>
       </c>
       <c r="OC399" t="n">
-        <v>25.47235133483689</v>
+        <v>38.33101307445015</v>
       </c>
       <c r="OD399" t="n">
-        <v>29.62651857687093</v>
+        <v>40.89556321980829</v>
       </c>
       <c r="OE399" t="n">
-        <v>29.30427807982484</v>
+        <v>39.4010210041742</v>
       </c>
       <c r="OF399" t="n">
-        <v>16.60583853585631</v>
+        <v>3.675036839084714</v>
       </c>
       <c r="OG399" t="n">
-        <v>16.61671967024451</v>
+        <v>4.254473041096979</v>
       </c>
       <c r="OH399" t="n">
         <v>0</v>
       </c>
       <c r="OI399" t="n">
-        <v>22.90311052323981</v>
+        <v>12.98455549470448</v>
       </c>
       <c r="OJ399" t="n">
-        <v>17.23653034214032</v>
+        <v>11.71412155455562</v>
       </c>
       <c r="OK399" t="n">
-        <v>19.14275431731421</v>
+        <v>6.581703187556073</v>
       </c>
       <c r="OL399" t="n">
-        <v>12.44565187452578</v>
+        <v>24.01203059444958</v>
       </c>
       <c r="OM399" t="n">
-        <v>15.81785179853036</v>
+        <v>28.7438863245746</v>
       </c>
       <c r="ON399" t="n">
-        <v>17.87427451976542</v>
+        <v>28.39305587534511</v>
       </c>
       <c r="OO399" t="n">
-        <v>16.20146278469587</v>
+        <v>8.392791713291283</v>
       </c>
       <c r="OP399" t="n">
-        <v>19.65234334646166</v>
+        <v>20.44825078029385</v>
       </c>
       <c r="OQ399" t="n">
-        <v>33.54079649383966</v>
+        <v>20.69666967946638</v>
       </c>
       <c r="OR399" t="n">
-        <v>40.94742320870991</v>
+        <v>28.54480970593324</v>
       </c>
       <c r="OS399" t="n">
-        <v>52.93868082562449</v>
+        <v>40.5417422123842</v>
       </c>
       <c r="OT399" t="n">
-        <v>23.13051447619125</v>
+        <v>15.66179069341616</v>
       </c>
       <c r="OU399" t="n">
-        <v>12.53494662622906</v>
+        <v>14.95022761715193</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="4" t="n"/>
       <c r="B400" s="1" t="inlineStr">
         <is>
-          <t>47100</t>
+          <t>47000</t>
         </is>
       </c>
       <c r="MX400" t="n">
-        <v>11.35166229401295</v>
+        <v>16.21018312729053</v>
       </c>
       <c r="MY400" t="n">
-        <v>17.68723551524109</v>
+        <v>22.53598413109489</v>
       </c>
       <c r="MZ400" t="n">
-        <v>23.46182754811851</v>
+        <v>29.97322818725198</v>
       </c>
       <c r="NA400" t="n">
-        <v>29.34264534101995</v>
+        <v>22.48269686097515</v>
       </c>
       <c r="NB400" t="n">
-        <v>18.18628628797919</v>
+        <v>19.52534461388999</v>
       </c>
       <c r="NC400" t="n">
-        <v>18.55215385156283</v>
+        <v>34.82916309582932</v>
       </c>
       <c r="ND400" t="n">
-        <v>18.72015841744752</v>
+        <v>37.74544411887438</v>
       </c>
       <c r="NE400" t="n">
-        <v>24.71780185812595</v>
+        <v>44.79546248013963</v>
       </c>
       <c r="NF400" t="n">
-        <v>38.6482971102602</v>
+        <v>60.74185755383225</v>
       </c>
       <c r="NG400" t="n">
-        <v>31.95305628141752</v>
+        <v>40.16156165562674</v>
       </c>
       <c r="NH400" t="n">
-        <v>38.98908800431567</v>
+        <v>40.29305415573404</v>
       </c>
       <c r="NI400" t="n">
-        <v>30.85611536596489</v>
+        <v>45.04246982006463</v>
       </c>
       <c r="NJ400" t="n">
-        <v>20.27066953513307</v>
+        <v>34.49295067553533</v>
       </c>
       <c r="NK400" t="n">
-        <v>24.2985464750796</v>
+        <v>29.16732727737413</v>
       </c>
       <c r="NL400" t="n">
-        <v>17.79182961251228</v>
+        <v>28.90147295331241</v>
       </c>
       <c r="NM400" t="n">
-        <v>11.28392456572946</v>
+        <v>26.06804239617902</v>
       </c>
       <c r="NN400" t="n">
-        <v>11.21628135258284</v>
+        <v>28.71641400908567</v>
       </c>
       <c r="NO400" t="n">
-        <v>27.42834277576236</v>
+        <v>42.62568333374519</v>
       </c>
       <c r="NP400" t="n">
-        <v>18.99037560631989</v>
+        <v>36.94075662161105</v>
       </c>
       <c r="NQ400" t="n">
-        <v>33.19188333205473</v>
+        <v>50.84126379819114</v>
       </c>
       <c r="NR400" t="n">
-        <v>38.78309515427254</v>
+        <v>61.30172596624892</v>
       </c>
       <c r="NS400" t="n">
-        <v>42.30439350309043</v>
+        <v>65.12966413426869</v>
       </c>
       <c r="NT400" t="n">
-        <v>62.03324767597061</v>
+        <v>40.6890833057524</v>
       </c>
       <c r="NU400" t="n">
-        <v>54.47492031097266</v>
+        <v>32.85135757465112</v>
       </c>
       <c r="NV400" t="n">
-        <v>51.06281255339238</v>
+        <v>30.10236587932901</v>
       </c>
       <c r="NW400" t="n">
-        <v>54.25382741118214</v>
+        <v>37.9170679558581</v>
       </c>
       <c r="NX400" t="n">
-        <v>121.676879104274</v>
+        <v>102.1998048761191</v>
       </c>
       <c r="NY400" t="n">
-        <v>109.1975723454027</v>
+        <v>89.53937196418444</v>
       </c>
       <c r="NZ400" t="n">
-        <v>101.1614410411764</v>
+        <v>82.43132347787902</v>
       </c>
       <c r="OA400" t="n">
-        <v>78.76477412478872</v>
+        <v>60.98371688216066</v>
       </c>
       <c r="OB400" t="n">
-        <v>66.49901658305473</v>
+        <v>49.22669048065715</v>
       </c>
       <c r="OC400" t="n">
-        <v>46.6626263527158</v>
+        <v>25.47235133483689</v>
       </c>
       <c r="OD400" t="n">
-        <v>46.41352920164212</v>
+        <v>29.62651857687093</v>
       </c>
       <c r="OE400" t="n">
-        <v>43.63099265649031</v>
+        <v>29.30427807982484</v>
       </c>
       <c r="OF400" t="n">
-        <v>10.07506377552812</v>
+        <v>16.60583853585631</v>
       </c>
       <c r="OG400" t="n">
-        <v>7.525252220864362</v>
+        <v>16.61671967024451</v>
       </c>
       <c r="OH400" t="n">
-        <v>22.90311052323981</v>
+        <v>12.98455549470448</v>
       </c>
       <c r="OI400" t="n">
         <v>0</v>
       </c>
       <c r="OJ400" t="n">
-        <v>5.690054496671892</v>
+        <v>22.90311052323981</v>
       </c>
       <c r="OK400" t="n">
-        <v>10.58334011603933</v>
+        <v>17.23653034214032</v>
       </c>
       <c r="OL400" t="n">
-        <v>34.96764633931125</v>
+        <v>12.44565187452578</v>
       </c>
       <c r="OM400" t="n">
-        <v>37.59694896763356</v>
+        <v>15.81785179853036</v>
       </c>
       <c r="ON400" t="n">
-        <v>39.75438057255388</v>
+        <v>17.87427451976542</v>
       </c>
       <c r="OO400" t="n">
-        <v>18.11924720673903</v>
+        <v>16.20146278469587</v>
       </c>
       <c r="OP400" t="n">
-        <v>31.52322651979821</v>
+        <v>19.65234147891611</v>
       </c>
       <c r="OQ400" t="n">
-        <v>12.65570835805011</v>
+        <v>33.54079649383966</v>
       </c>
       <c r="OR400" t="n">
-        <v>18.37893016264559</v>
+        <v>40.94742320870991</v>
       </c>
       <c r="OS400" t="n">
-        <v>30.23785755847216</v>
+        <v>52.93868082562449</v>
       </c>
       <c r="OT400" t="n">
-        <v>23.39598506867734</v>
+        <v>23.13051447619125</v>
       </c>
       <c r="OU400" t="n">
-        <v>26.58818136261413</v>
+        <v>12.53494662622906</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="4" t="n"/>
       <c r="B401" s="1" t="inlineStr">
         <is>
-          <t>47200</t>
+          <t>47100</t>
         </is>
       </c>
       <c r="MX401" t="n">
-        <v>8.437881867951438</v>
+        <v>11.35166229401295</v>
       </c>
       <c r="MY401" t="n">
-        <v>16.6756429456996</v>
+        <v>17.68723551524109</v>
       </c>
       <c r="MZ401" t="n">
-        <v>23.66057349296401</v>
+        <v>23.46182754811851</v>
       </c>
       <c r="NA401" t="n">
-        <v>26.36791892396908</v>
+        <v>29.34264534101995</v>
       </c>
       <c r="NB401" t="n">
-        <v>16.0967323701332</v>
+        <v>18.18628628797919</v>
       </c>
       <c r="NC401" t="n">
-        <v>21.84110241705717</v>
+        <v>18.55215385156283</v>
       </c>
       <c r="ND401" t="n">
-        <v>23.06166008731209</v>
+        <v>18.72015841744752</v>
       </c>
       <c r="NE401" t="n">
-        <v>29.55060030516367</v>
+        <v>24.71780185812595</v>
       </c>
       <c r="NF401" t="n">
-        <v>44.17487967756728</v>
+        <v>38.6482971102602</v>
       </c>
       <c r="NG401" t="n">
-        <v>33.14604671893554</v>
+        <v>31.95305628141752</v>
       </c>
       <c r="NH401" t="n">
-        <v>38.49877305186358</v>
+        <v>38.98908800431567</v>
       </c>
       <c r="NI401" t="n">
-        <v>33.86261225204071</v>
+        <v>30.85611536596489</v>
       </c>
       <c r="NJ401" t="n">
-        <v>22.10879446117209</v>
+        <v>20.27066953513307</v>
       </c>
       <c r="NK401" t="n">
-        <v>23.15619140503483</v>
+        <v>24.2985464750796</v>
       </c>
       <c r="NL401" t="n">
-        <v>15.97453919839341</v>
+        <v>18.7807116137732</v>
       </c>
       <c r="NM401" t="n">
-        <v>12.50847451243204</v>
+        <v>11.28392456572946</v>
       </c>
       <c r="NN401" t="n">
-        <v>13.85254185978611</v>
+        <v>11.21628135258284</v>
       </c>
       <c r="NO401" t="n">
-        <v>29.9377644219226</v>
+        <v>27.42834277576236</v>
       </c>
       <c r="NP401" t="n">
-        <v>22.30601128599626</v>
+        <v>18.99037560631989</v>
       </c>
       <c r="NQ401" t="n">
-        <v>36.72072096514074</v>
+        <v>33.19188333205473</v>
       </c>
       <c r="NR401" t="n">
-        <v>44.23593889549402</v>
+        <v>38.78309515427254</v>
       </c>
       <c r="NS401" t="n">
-        <v>47.91229503048633</v>
+        <v>42.30439350309043</v>
       </c>
       <c r="NT401" t="n">
-        <v>56.49159858256399</v>
+        <v>62.03324767597061</v>
       </c>
       <c r="NU401" t="n">
-        <v>48.88623503507016</v>
+        <v>54.47492031097266</v>
       </c>
       <c r="NV401" t="n">
-        <v>45.54630745009298</v>
+        <v>51.06281255339238</v>
       </c>
       <c r="NW401" t="n">
-        <v>50.01030693742152</v>
+        <v>54.25382741118214</v>
       </c>
       <c r="NX401" t="n">
-        <v>116.9626044099027</v>
+        <v>121.676879104274</v>
       </c>
       <c r="NY401" t="n">
-        <v>104.4238666042248</v>
+        <v>109.1975723454027</v>
       </c>
       <c r="NZ401" t="n">
-        <v>96.59911568215772</v>
+        <v>101.1614410411764</v>
       </c>
       <c r="OA401" t="n">
-        <v>74.36290386549057</v>
+        <v>78.76477412478872</v>
       </c>
       <c r="OB401" t="n">
-        <v>62.15216493368043</v>
+        <v>66.49901658305473</v>
       </c>
       <c r="OC401" t="n">
-        <v>41.38730691393158</v>
+        <v>46.6626263527158</v>
       </c>
       <c r="OD401" t="n">
-        <v>41.98360572437431</v>
+        <v>46.41352920164212</v>
       </c>
       <c r="OE401" t="n">
-        <v>39.64248690013154</v>
+        <v>43.63099265649031</v>
       </c>
       <c r="OF401" t="n">
-        <v>6.422484399208642</v>
+        <v>10.07506377552812</v>
       </c>
       <c r="OG401" t="n">
-        <v>3.211258392999594</v>
+        <v>7.525252220864362</v>
       </c>
       <c r="OH401" t="n">
-        <v>17.23653034214032</v>
+        <v>11.71412155455562</v>
       </c>
       <c r="OI401" t="n">
-        <v>5.690054496671892</v>
+        <v>22.90311052323981</v>
       </c>
       <c r="OJ401" t="n">
         <v>0</v>
       </c>
       <c r="OK401" t="n">
-        <v>8.343414447184793</v>
+        <v>5.690054496671892</v>
       </c>
       <c r="OL401" t="n">
-        <v>29.28050021940699</v>
+        <v>34.96764633931125</v>
       </c>
       <c r="OM401" t="n">
-        <v>32.16456105084714</v>
+        <v>37.59694896763356</v>
       </c>
       <c r="ON401" t="n">
-        <v>34.11129926978727</v>
+        <v>39.75438057255388</v>
       </c>
       <c r="OO401" t="n">
-        <v>14.24987010067157</v>
+        <v>18.11924720673903</v>
       </c>
       <c r="OP401" t="n">
-        <v>26.98494587320598</v>
+        <v>31.52322564830138</v>
       </c>
       <c r="OQ401" t="n">
-        <v>17.15252249939733</v>
+        <v>12.65570835805011</v>
       </c>
       <c r="OR401" t="n">
-        <v>23.82598940813596</v>
+        <v>18.37893016264559</v>
       </c>
       <c r="OS401" t="n">
-        <v>35.77266091826494</v>
+        <v>30.23785755847216</v>
       </c>
       <c r="OT401" t="n">
-        <v>20.70355057081901</v>
+        <v>23.39598506867734</v>
       </c>
       <c r="OU401" t="n">
-        <v>21.49429916321459</v>
+        <v>26.58818136261413</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="4" t="n"/>
       <c r="B402" s="1" t="inlineStr">
         <is>
-          <t>47810</t>
+          <t>47200</t>
         </is>
       </c>
       <c r="MX402" t="n">
-        <v>16.49158977239168</v>
+        <v>8.437881867951438</v>
       </c>
       <c r="MY402" t="n">
-        <v>24.98017908834223</v>
+        <v>16.6756429456996</v>
       </c>
       <c r="MZ402" t="n">
-        <v>31.99629414795935</v>
+        <v>23.66057349296401</v>
       </c>
       <c r="NA402" t="n">
-        <v>33.70778025680086</v>
+        <v>26.36791892396908</v>
       </c>
       <c r="NB402" t="n">
-        <v>24.15659938104967</v>
+        <v>16.0967323701332</v>
       </c>
       <c r="NC402" t="n">
-        <v>29.03379155698689</v>
+        <v>21.84110241705717</v>
       </c>
       <c r="ND402" t="n">
-        <v>29.26630511125472</v>
+        <v>23.06166008731209</v>
       </c>
       <c r="NE402" t="n">
-        <v>34.99698929754675</v>
+        <v>29.55060030516367</v>
       </c>
       <c r="NF402" t="n">
-        <v>47.53945438684443</v>
+        <v>44.17487967756728</v>
       </c>
       <c r="NG402" t="n">
-        <v>41.36892776554819</v>
+        <v>33.14604671893554</v>
       </c>
       <c r="NH402" t="n">
-        <v>46.79405227604212</v>
+        <v>38.49877305186358</v>
       </c>
       <c r="NI402" t="n">
-        <v>41.29794527824796</v>
+        <v>33.86261225204071</v>
       </c>
       <c r="NJ402" t="n">
-        <v>15.67548064326493</v>
+        <v>22.10879446117209</v>
       </c>
       <c r="NK402" t="n">
-        <v>14.81615330492677</v>
+        <v>23.15619140503483</v>
       </c>
       <c r="NL402" t="n">
-        <v>7.656945560449512</v>
+        <v>18.91808199046341</v>
       </c>
       <c r="NM402" t="n">
-        <v>6.957618606044848</v>
+        <v>12.50847451243204</v>
       </c>
       <c r="NN402" t="n">
-        <v>9.860401371793374</v>
+        <v>13.85254185978611</v>
       </c>
       <c r="NO402" t="n">
-        <v>23.83479221606745</v>
+        <v>29.9377644219226</v>
       </c>
       <c r="NP402" t="n">
-        <v>17.82047071984808</v>
+        <v>22.30601128599626</v>
       </c>
       <c r="NQ402" t="n">
-        <v>31.74395861357146</v>
+        <v>36.72072096514074</v>
       </c>
       <c r="NR402" t="n">
-        <v>43.64777934861662</v>
+        <v>44.23593889549402</v>
       </c>
       <c r="NS402" t="n">
-        <v>48.1870961165827</v>
+        <v>47.91229503048633</v>
       </c>
       <c r="NT402" t="n">
-        <v>54.23499867426946</v>
+        <v>56.49159858256399</v>
       </c>
       <c r="NU402" t="n">
-        <v>47.05538344664005</v>
+        <v>48.88623503507016</v>
       </c>
       <c r="NV402" t="n">
-        <v>43.24954028262403</v>
+        <v>45.54630745009298</v>
       </c>
       <c r="NW402" t="n">
-        <v>55.52154840889894</v>
+        <v>50.01030693742152</v>
       </c>
       <c r="NX402" t="n">
-        <v>121.1990960452153</v>
+        <v>116.9626044099027</v>
       </c>
       <c r="NY402" t="n">
-        <v>108.5604948329179</v>
+        <v>104.4238666042248</v>
       </c>
       <c r="NZ402" t="n">
-        <v>101.2251075185475</v>
+        <v>96.59911568215772</v>
       </c>
       <c r="OA402" t="n">
-        <v>79.4020145729573</v>
+        <v>74.36290386549057</v>
       </c>
       <c r="OB402" t="n">
-        <v>67.37285204182045</v>
+        <v>62.15216493368043</v>
       </c>
       <c r="OC402" t="n">
-        <v>44.59697608130264</v>
+        <v>41.38730691393158</v>
       </c>
       <c r="OD402" t="n">
-        <v>47.28633800481356</v>
+        <v>41.98360572437431</v>
       </c>
       <c r="OE402" t="n">
-        <v>45.67676240665195</v>
+        <v>39.64248690013154</v>
       </c>
       <c r="OF402" t="n">
-        <v>2.834429869728361</v>
+        <v>6.422484399208642</v>
       </c>
       <c r="OG402" t="n">
-        <v>5.339553017252469</v>
+        <v>3.211258392999594</v>
       </c>
       <c r="OH402" t="n">
-        <v>19.14275431731421</v>
+        <v>6.581703187556073</v>
       </c>
       <c r="OI402" t="n">
-        <v>10.58334011603933</v>
+        <v>17.23653034214032</v>
       </c>
       <c r="OJ402" t="n">
-        <v>8.343414447184793</v>
+        <v>5.690054496671892</v>
       </c>
       <c r="OK402" t="n">
         <v>0</v>
       </c>
       <c r="OL402" t="n">
-        <v>29.29959425738851</v>
+        <v>29.28050021940699</v>
       </c>
       <c r="OM402" t="n">
-        <v>34.95968724418567</v>
+        <v>32.16456105084714</v>
       </c>
       <c r="ON402" t="n">
-        <v>33.09627788356254</v>
+        <v>34.11129926978727</v>
       </c>
       <c r="OO402" t="n">
-        <v>8.028895418786716</v>
+        <v>14.24987010067157</v>
       </c>
       <c r="OP402" t="n">
-        <v>21.68637633856127</v>
+        <v>26.98494480218243</v>
       </c>
       <c r="OQ402" t="n">
-        <v>15.51829985077686</v>
+        <v>17.15252249939733</v>
       </c>
       <c r="OR402" t="n">
-        <v>24.03228874165542</v>
+        <v>23.82598940813596</v>
       </c>
       <c r="OS402" t="n">
-        <v>35.83625789693938</v>
+        <v>35.77266091826494</v>
       </c>
       <c r="OT402" t="n">
-        <v>12.85496992057921</v>
+        <v>20.70355057081901</v>
       </c>
       <c r="OU402" t="n">
-        <v>17.95031266696045</v>
+        <v>21.49429916321459</v>
       </c>
     </row>
     <row r="403">
@@ -56386,7 +56386,7 @@
         <v>35.12914138540963</v>
       </c>
       <c r="NL403" t="n">
-        <v>30.51551524989133</v>
+        <v>37.01711659437225</v>
       </c>
       <c r="NM403" t="n">
         <v>36.15343498079947</v>
@@ -56452,16 +56452,16 @@
         <v>28.10505186291871</v>
       </c>
       <c r="OH403" t="n">
+        <v>24.01203059444958</v>
+      </c>
+      <c r="OI403" t="n">
         <v>12.44565187452578</v>
       </c>
-      <c r="OI403" t="n">
+      <c r="OJ403" t="n">
         <v>34.96764633931125</v>
       </c>
-      <c r="OJ403" t="n">
+      <c r="OK403" t="n">
         <v>29.28050021940699</v>
-      </c>
-      <c r="OK403" t="n">
-        <v>29.29959425738851</v>
       </c>
       <c r="OL403" t="n">
         <v>0</v>
@@ -56476,7 +56476,7 @@
         <v>23.64084280723874</v>
       </c>
       <c r="OP403" t="n">
-        <v>18.72342013909966</v>
+        <v>18.72341830888853</v>
       </c>
       <c r="OQ403" t="n">
         <v>44.59898507709013</v>
@@ -56544,7 +56544,7 @@
         <v>43.94614283969175</v>
       </c>
       <c r="NL404" t="n">
-        <v>38.22059816726475</v>
+        <v>44.48379375656454</v>
       </c>
       <c r="NM404" t="n">
         <v>41.8761217576691</v>
@@ -56610,16 +56610,16 @@
         <v>32.11945293415265</v>
       </c>
       <c r="OH404" t="n">
+        <v>28.7438863245746</v>
+      </c>
+      <c r="OI404" t="n">
         <v>15.81785179853036</v>
       </c>
-      <c r="OI404" t="n">
+      <c r="OJ404" t="n">
         <v>37.59694896763356</v>
       </c>
-      <c r="OJ404" t="n">
+      <c r="OK404" t="n">
         <v>32.16456105084714</v>
-      </c>
-      <c r="OK404" t="n">
-        <v>34.95968724418567</v>
       </c>
       <c r="OL404" t="n">
         <v>11.42844566343307</v>
@@ -56634,7 +56634,7 @@
         <v>31.33949327586451</v>
       </c>
       <c r="OP404" t="n">
-        <v>29.63282560738857</v>
+        <v>29.63282369729135</v>
       </c>
       <c r="OQ404" t="n">
         <v>49.0404449207352</v>
@@ -56702,7 +56702,7 @@
         <v>36.77269409929857</v>
       </c>
       <c r="NL405" t="n">
-        <v>33.13215229355873</v>
+        <v>39.60467335755997</v>
       </c>
       <c r="NM405" t="n">
         <v>39.7331306059278</v>
@@ -56768,16 +56768,16 @@
         <v>32.60510591652795</v>
       </c>
       <c r="OH405" t="n">
+        <v>28.39305587534511</v>
+      </c>
+      <c r="OI405" t="n">
         <v>17.87427451976542</v>
       </c>
-      <c r="OI405" t="n">
+      <c r="OJ405" t="n">
         <v>39.75438057255388</v>
       </c>
-      <c r="OJ405" t="n">
+      <c r="OK405" t="n">
         <v>34.11129926978727</v>
-      </c>
-      <c r="OK405" t="n">
-        <v>33.09627788356254</v>
       </c>
       <c r="OL405" t="n">
         <v>5.840742869708822</v>
@@ -56792,7 +56792,7 @@
         <v>26.55046416338517</v>
       </c>
       <c r="OP405" t="n">
-        <v>18.48397862165317</v>
+        <v>18.48397709424696</v>
       </c>
       <c r="OQ405" t="n">
         <v>48.59211951854623</v>
@@ -56860,7 +56860,7 @@
         <v>12.99278057532591</v>
       </c>
       <c r="NL406" t="n">
-        <v>6.944829349184612</v>
+        <v>13.40173829585335</v>
       </c>
       <c r="NM406" t="n">
         <v>13.57199049330612</v>
@@ -56926,16 +56926,16 @@
         <v>11.13665910404527</v>
       </c>
       <c r="OH406" t="n">
+        <v>8.392791713291283</v>
+      </c>
+      <c r="OI406" t="n">
         <v>16.20146278469587</v>
       </c>
-      <c r="OI406" t="n">
+      <c r="OJ406" t="n">
         <v>18.11924720673903</v>
       </c>
-      <c r="OJ406" t="n">
+      <c r="OK406" t="n">
         <v>14.24987010067157</v>
-      </c>
-      <c r="OK406" t="n">
-        <v>8.028895418786716</v>
       </c>
       <c r="OL406" t="n">
         <v>23.64084280723874</v>
@@ -56950,7 +56950,7 @@
         <v>0</v>
       </c>
       <c r="OP406" t="n">
-        <v>13.65773369653359</v>
+        <v>13.65773308842921</v>
       </c>
       <c r="OQ406" t="n">
         <v>22.94598033051579</v>
@@ -56976,154 +56976,154 @@
         </is>
       </c>
       <c r="MX407" t="n">
-        <v>31.53198498237143</v>
+        <v>31.53198354764007</v>
       </c>
       <c r="MY407" t="n">
-        <v>39.79160000162474</v>
+        <v>39.7915984616263</v>
       </c>
       <c r="MZ407" t="n">
-        <v>47.53257583985823</v>
+        <v>47.53257429788042</v>
       </c>
       <c r="NA407" t="n">
-        <v>42.1074057529838</v>
+        <v>42.10740390920709</v>
       </c>
       <c r="NB407" t="n">
-        <v>37.39253186264108</v>
+        <v>37.3925302514103</v>
       </c>
       <c r="NC407" t="n">
-        <v>48.71618362833904</v>
+        <v>48.71618246062985</v>
       </c>
       <c r="ND407" t="n">
-        <v>49.99644238330549</v>
+        <v>49.99644138086828</v>
       </c>
       <c r="NE407" t="n">
-        <v>56.23729982546006</v>
+        <v>56.23729893616719</v>
       </c>
       <c r="NF407" t="n">
-        <v>69.20704454708716</v>
+        <v>69.20704401037412</v>
       </c>
       <c r="NG407" t="n">
-        <v>57.76399693502781</v>
+        <v>57.76399541271257</v>
       </c>
       <c r="NH407" t="n">
-        <v>59.51713958859602</v>
+        <v>59.51713784702827</v>
       </c>
       <c r="NI407" t="n">
-        <v>60.44259043512652</v>
+        <v>60.44258916207625</v>
       </c>
       <c r="NJ407" t="n">
-        <v>30.26586040541633</v>
+        <v>30.26586080376381</v>
       </c>
       <c r="NK407" t="n">
-        <v>19.37021805527369</v>
+        <v>19.37021884787363</v>
       </c>
       <c r="NL407" t="n">
-        <v>18.02967411192094</v>
+        <v>23.81138292074619</v>
       </c>
       <c r="NM407" t="n">
-        <v>26.64392671010039</v>
+        <v>26.6439264970733</v>
       </c>
       <c r="NN407" t="n">
-        <v>29.91019958808815</v>
+        <v>29.91019939562835</v>
       </c>
       <c r="NO407" t="n">
-        <v>36.87240344349247</v>
+        <v>36.8724041120022</v>
       </c>
       <c r="NP407" t="n">
-        <v>35.37687317001358</v>
+        <v>35.37687336944715</v>
       </c>
       <c r="NQ407" t="n">
-        <v>46.05921695660545</v>
+        <v>46.0592176131961</v>
       </c>
       <c r="NR407" t="n">
-        <v>63.37109996089509</v>
+        <v>63.37110003574004</v>
       </c>
       <c r="NS407" t="n">
-        <v>68.51446648254252</v>
+        <v>68.51446644979339</v>
       </c>
       <c r="NT407" t="n">
-        <v>34.63154950022449</v>
+        <v>34.63154901959135</v>
       </c>
       <c r="NU407" t="n">
-        <v>28.53292590380833</v>
+        <v>28.53292512797516</v>
       </c>
       <c r="NV407" t="n">
-        <v>24.19057487955794</v>
+        <v>24.19057417526572</v>
       </c>
       <c r="NW407" t="n">
-        <v>54.50507807783873</v>
+        <v>54.50507614813898</v>
       </c>
       <c r="NX407" t="n">
-        <v>113.2276508301453</v>
+        <v>113.2276492183155</v>
       </c>
       <c r="NY407" t="n">
-        <v>100.5896680480641</v>
+        <v>100.5896664243062</v>
       </c>
       <c r="NZ407" t="n">
-        <v>94.87967703466988</v>
+        <v>94.87967532092564</v>
       </c>
       <c r="OA407" t="n">
-        <v>75.17025999515091</v>
+        <v>75.1702581719654</v>
       </c>
       <c r="OB407" t="n">
-        <v>64.42567892847572</v>
+        <v>64.42567705161842</v>
       </c>
       <c r="OC407" t="n">
-        <v>38.25673170115465</v>
+        <v>38.25672986206825</v>
       </c>
       <c r="OD407" t="n">
-        <v>46.58042536441588</v>
+        <v>46.58042342171095</v>
       </c>
       <c r="OE407" t="n">
-        <v>47.55016400369718</v>
+        <v>47.55016204892787</v>
       </c>
       <c r="OF407" t="n">
-        <v>21.45953749051091</v>
+        <v>21.45953665135958</v>
       </c>
       <c r="OG407" t="n">
-        <v>24.16687687868328</v>
+        <v>24.1668759081573</v>
       </c>
       <c r="OH407" t="n">
-        <v>19.65234334646166</v>
+        <v>20.44825078029385</v>
       </c>
       <c r="OI407" t="n">
-        <v>31.52322651979821</v>
+        <v>19.65234147891611</v>
       </c>
       <c r="OJ407" t="n">
-        <v>26.98494587320598</v>
+        <v>31.52322564830138</v>
       </c>
       <c r="OK407" t="n">
-        <v>21.68637633856127</v>
+        <v>26.98494480218243</v>
       </c>
       <c r="OL407" t="n">
-        <v>18.72342013909966</v>
+        <v>18.72341830888853</v>
       </c>
       <c r="OM407" t="n">
-        <v>29.63282560738857</v>
+        <v>29.63282369729135</v>
       </c>
       <c r="ON407" t="n">
-        <v>18.48397862165317</v>
+        <v>18.48397709424696</v>
       </c>
       <c r="OO407" t="n">
-        <v>13.65773369653359</v>
+        <v>13.65773308842921</v>
       </c>
       <c r="OP407" t="n">
         <v>0</v>
       </c>
       <c r="OQ407" t="n">
-        <v>36.1486507024518</v>
+        <v>36.14865048528043</v>
       </c>
       <c r="OR407" t="n">
-        <v>45.0315426538475</v>
+        <v>45.03154240083416</v>
       </c>
       <c r="OS407" t="n">
-        <v>56.32021019850686</v>
+        <v>56.32021010379893</v>
       </c>
       <c r="OT407" t="n">
-        <v>13.01045568922131</v>
+        <v>13.01045619152112</v>
       </c>
       <c r="OU407" t="n">
-        <v>7.157608871707878</v>
+        <v>7.157607059650623</v>
       </c>
     </row>
     <row r="408">
@@ -57176,7 +57176,7 @@
         <v>21.7440095845571</v>
       </c>
       <c r="NL408" t="n">
-        <v>18.47040353933542</v>
+        <v>14.88661294438268</v>
       </c>
       <c r="NM408" t="n">
         <v>9.504954504205804</v>
@@ -57242,16 +57242,16 @@
         <v>16.94489140394498</v>
       </c>
       <c r="OH408" t="n">
+        <v>20.69666967946638</v>
+      </c>
+      <c r="OI408" t="n">
         <v>33.54079649383966</v>
       </c>
-      <c r="OI408" t="n">
+      <c r="OJ408" t="n">
         <v>12.65570835805011</v>
       </c>
-      <c r="OJ408" t="n">
+      <c r="OK408" t="n">
         <v>17.15252249939733</v>
-      </c>
-      <c r="OK408" t="n">
-        <v>15.51829985077686</v>
       </c>
       <c r="OL408" t="n">
         <v>44.59898507709013</v>
@@ -57266,7 +57266,7 @@
         <v>22.94598033051579</v>
       </c>
       <c r="OP408" t="n">
-        <v>36.1486507024518</v>
+        <v>36.14865048528043</v>
       </c>
       <c r="OQ408" t="n">
         <v>0</v>
@@ -57334,7 +57334,7 @@
         <v>30.2209586783266</v>
       </c>
       <c r="NL409" t="n">
-        <v>27.37873787599867</v>
+        <v>23.41444484645461</v>
       </c>
       <c r="NM409" t="n">
         <v>18.40145878245156</v>
@@ -57400,16 +57400,16 @@
         <v>24.46554114371723</v>
       </c>
       <c r="OH409" t="n">
+        <v>28.54480970593324</v>
+      </c>
+      <c r="OI409" t="n">
         <v>40.94742320870991</v>
       </c>
-      <c r="OI409" t="n">
+      <c r="OJ409" t="n">
         <v>18.37893016264559</v>
       </c>
-      <c r="OJ409" t="n">
+      <c r="OK409" t="n">
         <v>23.82598940813596</v>
-      </c>
-      <c r="OK409" t="n">
-        <v>24.03228874165542</v>
       </c>
       <c r="OL409" t="n">
         <v>52.54947933970337</v>
@@ -57424,7 +57424,7 @@
         <v>31.71205146685969</v>
       </c>
       <c r="OP409" t="n">
-        <v>45.0315426538475</v>
+        <v>45.03154240083416</v>
       </c>
       <c r="OQ409" t="n">
         <v>8.914092658531199</v>
@@ -57492,7 +57492,7 @@
         <v>39.97376413080153</v>
       </c>
       <c r="NL410" t="n">
-        <v>38.37050164766071</v>
+        <v>33.50643538169317</v>
       </c>
       <c r="NM410" t="n">
         <v>29.76933974964478</v>
@@ -57558,16 +57558,16 @@
         <v>36.47369612058229</v>
       </c>
       <c r="OH410" t="n">
+        <v>40.5417422123842</v>
+      </c>
+      <c r="OI410" t="n">
         <v>52.93868082562449</v>
       </c>
-      <c r="OI410" t="n">
+      <c r="OJ410" t="n">
         <v>30.23785755847216</v>
       </c>
-      <c r="OJ410" t="n">
+      <c r="OK410" t="n">
         <v>35.77266091826494</v>
-      </c>
-      <c r="OK410" t="n">
-        <v>35.83625789693938</v>
       </c>
       <c r="OL410" t="n">
         <v>64.55126484077441</v>
@@ -57582,7 +57582,7 @@
         <v>43.30068076795123</v>
       </c>
       <c r="OP410" t="n">
-        <v>56.32021019850686</v>
+        <v>56.32021010379893</v>
       </c>
       <c r="OQ410" t="n">
         <v>20.369910421897</v>
@@ -57650,7 +57650,7 @@
         <v>6.833315300641224</v>
       </c>
       <c r="NL411" t="n">
-        <v>6.132986242918765</v>
+        <v>10.90709615854646</v>
       </c>
       <c r="NM411" t="n">
         <v>15.24975088967401</v>
@@ -57716,16 +57716,16 @@
         <v>17.49278491959333</v>
       </c>
       <c r="OH411" t="n">
+        <v>15.66179069341616</v>
+      </c>
+      <c r="OI411" t="n">
         <v>23.13051447619125</v>
       </c>
-      <c r="OI411" t="n">
+      <c r="OJ411" t="n">
         <v>23.39598506867734</v>
       </c>
-      <c r="OJ411" t="n">
+      <c r="OK411" t="n">
         <v>20.70355057081901</v>
-      </c>
-      <c r="OK411" t="n">
-        <v>12.85496992057921</v>
       </c>
       <c r="OL411" t="n">
         <v>28.32757819464436</v>
@@ -57740,7 +57740,7 @@
         <v>7.60268982958454</v>
       </c>
       <c r="OP411" t="n">
-        <v>13.01045568922131</v>
+        <v>13.01045619152112</v>
       </c>
       <c r="OQ411" t="n">
         <v>24.4834345571483</v>
@@ -57808,7 +57808,7 @@
         <v>20.87047111991753</v>
       </c>
       <c r="NL412" t="n">
-        <v>16.92699002249816</v>
+        <v>23.38478275615603</v>
       </c>
       <c r="NM412" t="n">
         <v>24.09105680659523</v>
@@ -57874,16 +57874,16 @@
         <v>19.06312688935055</v>
       </c>
       <c r="OH412" t="n">
+        <v>14.95022761715193</v>
+      </c>
+      <c r="OI412" t="n">
         <v>12.53494662622906</v>
       </c>
-      <c r="OI412" t="n">
+      <c r="OJ412" t="n">
         <v>26.58818136261413</v>
       </c>
-      <c r="OJ412" t="n">
+      <c r="OK412" t="n">
         <v>21.49429916321459</v>
-      </c>
-      <c r="OK412" t="n">
-        <v>17.95031266696045</v>
       </c>
       <c r="OL412" t="n">
         <v>14.30014620975612</v>
@@ -57898,7 +57898,7 @@
         <v>10.56809614706226</v>
       </c>
       <c r="OP412" t="n">
-        <v>7.157608871707878</v>
+        <v>7.157607059650623</v>
       </c>
       <c r="OQ412" t="n">
         <v>33.34297539386706</v>

</xml_diff>